<commit_message>
Changes for nonlinear propagation
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\course-repos\optimal-estimation-course\06-course-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC32BDF9-4F2E-46A7-8ED6-BBFD001B96DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47438A5-1E2B-0147-A0E0-5A27D56F6CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="14400" windowHeight="8190" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,21 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="268">
   <si>
     <t>Value</t>
   </si>
@@ -119,33 +129,12 @@
     <t>3-sigma steady-state gyro bias</t>
   </si>
   <si>
-    <t>del_gyrox</t>
-  </si>
-  <si>
-    <t>Injected gyro bias error</t>
-  </si>
-  <si>
-    <t>del_gyroy</t>
-  </si>
-  <si>
-    <t>del_gyroz</t>
-  </si>
-  <si>
-    <t>tau_gyro</t>
-  </si>
-  <si>
-    <t>Gyro bias ECRV time constant</t>
-  </si>
-  <si>
     <t>pos</t>
   </si>
   <si>
     <t>vel</t>
   </si>
   <si>
-    <t>att</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -275,12 +264,6 @@
     <t>gbias</t>
   </si>
   <si>
-    <t>stmis</t>
-  </si>
-  <si>
-    <t>cmis</t>
-  </si>
-  <si>
     <t>ri_x</t>
   </si>
   <si>
@@ -434,33 +417,6 @@
     <t>del_vsz</t>
   </si>
   <si>
-    <t>del_ax</t>
-  </si>
-  <si>
-    <t>del_ay</t>
-  </si>
-  <si>
-    <t>del_az</t>
-  </si>
-  <si>
-    <t>del_thstx</t>
-  </si>
-  <si>
-    <t>del_thsty</t>
-  </si>
-  <si>
-    <t>del_thstz</t>
-  </si>
-  <si>
-    <t>del_thcx</t>
-  </si>
-  <si>
-    <t>del_thcy</t>
-  </si>
-  <si>
-    <t>del_thcz</t>
-  </si>
-  <si>
     <t>W_MOON</t>
   </si>
   <si>
@@ -485,33 +441,6 @@
     <t>Injected satellite velocity error</t>
   </si>
   <si>
-    <t>Injected satellite orientation error</t>
-  </si>
-  <si>
-    <t>Injected star camera misalignment error</t>
-  </si>
-  <si>
-    <t>Injected terrain camera misalignment error</t>
-  </si>
-  <si>
-    <t>th_z</t>
-  </si>
-  <si>
-    <t>th_y</t>
-  </si>
-  <si>
-    <t>z angle of a ZYX euler angle sequence to define initial orientation of spacecraft</t>
-  </si>
-  <si>
-    <t>y angle of a ZYX euler angle sequence to define initial orientation of spacecraft</t>
-  </si>
-  <si>
-    <t>x angle of a ZYX euler angle sequence to define initial orientation of spacecraft</t>
-  </si>
-  <si>
-    <t>th_x</t>
-  </si>
-  <si>
     <t>n_MonteCarloRuns</t>
   </si>
   <si>
@@ -659,9 +588,6 @@
     <t>vo_diagnostics_enable</t>
   </si>
   <si>
-    <t>mrad</t>
-  </si>
-  <si>
     <t>use_approx_cam_attitude_change_enable</t>
   </si>
   <si>
@@ -672,6 +598,258 @@
   </si>
   <si>
     <t>flag to enable correlated Kalman update</t>
+  </si>
+  <si>
+    <t>b_r</t>
+  </si>
+  <si>
+    <t>epsilong_x</t>
+  </si>
+  <si>
+    <t>epsilong_y</t>
+  </si>
+  <si>
+    <t>epsilong_z</t>
+  </si>
+  <si>
+    <t>rf_x</t>
+  </si>
+  <si>
+    <t>rf_y</t>
+  </si>
+  <si>
+    <t>rf_z</t>
+  </si>
+  <si>
+    <t>h_t</t>
+  </si>
+  <si>
+    <t>ba_x</t>
+  </si>
+  <si>
+    <t>ba_y</t>
+  </si>
+  <si>
+    <t>ba_z</t>
+  </si>
+  <si>
+    <t>x component of bias in gravity of the moon</t>
+  </si>
+  <si>
+    <t>y component of bias in gravity of the moon</t>
+  </si>
+  <si>
+    <t>z component of bias in gravity of the moon</t>
+  </si>
+  <si>
+    <t>x component of the position of the observed feature</t>
+  </si>
+  <si>
+    <t>y component of the position of the observed feature</t>
+  </si>
+  <si>
+    <t>z component of the position of the observed feature</t>
+  </si>
+  <si>
+    <t>clock bias, seen as bias in the measured range</t>
+  </si>
+  <si>
+    <t>m/s^2</t>
+  </si>
+  <si>
+    <t>x component of bias in the accelerometer in the body frame</t>
+  </si>
+  <si>
+    <t>y component of bias in the accelerometer in the body frame</t>
+  </si>
+  <si>
+    <t>z component of bias in the accelerometer in the body frame</t>
+  </si>
+  <si>
+    <t>q_moon</t>
+  </si>
+  <si>
+    <t>q_camera</t>
+  </si>
+  <si>
+    <t>b_clock</t>
+  </si>
+  <si>
+    <t>pos_f</t>
+  </si>
+  <si>
+    <t>b_accl</t>
+  </si>
+  <si>
+    <t>b_accel</t>
+  </si>
+  <si>
+    <t>del_b</t>
+  </si>
+  <si>
+    <t>del_epsilong_x</t>
+  </si>
+  <si>
+    <t>del_epsilong_y</t>
+  </si>
+  <si>
+    <t>del_epsilong_z</t>
+  </si>
+  <si>
+    <t>del_h_t</t>
+  </si>
+  <si>
+    <t>del_b_accel_x</t>
+  </si>
+  <si>
+    <t>del_b_accel_y</t>
+  </si>
+  <si>
+    <t>del_b_accel_z</t>
+  </si>
+  <si>
+    <t>Injected clock bias error</t>
+  </si>
+  <si>
+    <t>Injected gravitational bias error</t>
+  </si>
+  <si>
+    <t>injected feature height error</t>
+  </si>
+  <si>
+    <t>injected accelerometer error</t>
+  </si>
+  <si>
+    <t>m/sec^2</t>
+  </si>
+  <si>
+    <t>qm_i_a</t>
+  </si>
+  <si>
+    <t>qm_i_i</t>
+  </si>
+  <si>
+    <t>qm_i_j</t>
+  </si>
+  <si>
+    <t>qm_i_k</t>
+  </si>
+  <si>
+    <t>qc_b_a</t>
+  </si>
+  <si>
+    <t>qc_b_i</t>
+  </si>
+  <si>
+    <t>qc_b_j</t>
+  </si>
+  <si>
+    <t>qc_b_k</t>
+  </si>
+  <si>
+    <t>real component of the orientation in the inertial frame with respect to the moon</t>
+  </si>
+  <si>
+    <t>i component of the orientation in the inertial frame with respect to the moon</t>
+  </si>
+  <si>
+    <t>j component of the orientation in the inertial frame with respect to the moon</t>
+  </si>
+  <si>
+    <t>k component of the orientation in the inertial frame with respect to the moon</t>
+  </si>
+  <si>
+    <t>scalar component of the orientation of the body frame with respect to the camera</t>
+  </si>
+  <si>
+    <t>i component of the orientation of the body frame with respect to the camera</t>
+  </si>
+  <si>
+    <t>j component of the orientation of the body frame with respect to the camera</t>
+  </si>
+  <si>
+    <t>k component of the orientation of the body frame with respect to the camera</t>
+  </si>
+  <si>
+    <t>initial height of the terrain relative to the reference sphere</t>
+  </si>
+  <si>
+    <t>tau_r</t>
+  </si>
+  <si>
+    <t>Range bias ECRV time constant</t>
+  </si>
+  <si>
+    <t>d_g</t>
+  </si>
+  <si>
+    <t>d_h</t>
+  </si>
+  <si>
+    <t>Distance correlation for height</t>
+  </si>
+  <si>
+    <t>astar_x_tf</t>
+  </si>
+  <si>
+    <t>Desired downrange acceleration at final time</t>
+  </si>
+  <si>
+    <t>astar_y_tf</t>
+  </si>
+  <si>
+    <t>Desired vertical acceleration at final time</t>
+  </si>
+  <si>
+    <t>vstar_x_tf</t>
+  </si>
+  <si>
+    <t>Desired downrange velocity at final time</t>
+  </si>
+  <si>
+    <t>vstar_y_tf</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Desired vertical velocity at final time</t>
+  </si>
+  <si>
+    <t>rstar_x_tf</t>
+  </si>
+  <si>
+    <t>Desired downrange position at final time</t>
+  </si>
+  <si>
+    <t>r0</t>
+  </si>
+  <si>
+    <t>Downrange location of landing site</t>
+  </si>
+  <si>
+    <t>tau_ax</t>
+  </si>
+  <si>
+    <t>Acceleration bias</t>
+  </si>
+  <si>
+    <t>seed_h</t>
+  </si>
+  <si>
+    <t>Seed for the terrain generator</t>
+  </si>
+  <si>
+    <t>astar_z_tf</t>
+  </si>
+  <si>
+    <t>vstar_z_tf</t>
+  </si>
+  <si>
+    <t>rstar_y_tf</t>
+  </si>
+  <si>
+    <t>rstar_z_tf</t>
   </si>
 </sst>
 </file>
@@ -684,7 +862,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,6 +874,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -844,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -874,7 +1059,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -894,8 +1078,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -920,6 +1102,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1258,80 +1452,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="64" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="E1" s="61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="62">
         <v>2</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="66">
+      <c r="E2" s="63">
         <f t="shared" ref="E2:E10" si="0">B2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="64">
         <v>0.25</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="68">
+        <v>54</v>
+      </c>
+      <c r="E3" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="67">
+        <v>40</v>
+      </c>
+      <c r="B4" s="64">
         <f>B5*0.5</f>
         <v>3404.7101009954345</v>
       </c>
@@ -1339,18 +1533,18 @@
         <v>5</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="68">
+        <v>55</v>
+      </c>
+      <c r="E4" s="65">
         <f t="shared" si="0"/>
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="67">
+        <v>41</v>
+      </c>
+      <c r="B5" s="64">
         <f>2*PI()/SQRT(B9)*((B11+B12+2*B13)/2)^(3/2)</f>
         <v>6809.4202019908689</v>
       </c>
@@ -1358,18 +1552,18 @@
         <v>5</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="68">
+        <v>56</v>
+      </c>
+      <c r="E5" s="65">
         <f>B5</f>
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="69">
+      <c r="B6" s="66">
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -1378,34 +1572,34 @@
       <c r="D6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="65">
         <f>B6</f>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="69">
+        <v>57</v>
+      </c>
+      <c r="B7" s="66">
         <v>15</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="68">
+        <v>58</v>
+      </c>
+      <c r="E7" s="65">
         <f>B7</f>
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="69">
+        <v>131</v>
+      </c>
+      <c r="B8" s="66">
         <f>12*6</f>
         <v>72</v>
       </c>
@@ -1415,271 +1609,271 @@
       <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="65">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="70">
+        <v>42</v>
+      </c>
+      <c r="B9" s="67">
         <v>4902.8010759999997</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="68">
+        <v>59</v>
+      </c>
+      <c r="E9" s="65">
         <f>B9*1000^3</f>
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="67">
+        <v>43</v>
+      </c>
+      <c r="B10" s="64">
         <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="68">
+        <v>60</v>
+      </c>
+      <c r="E10" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="67">
+        <v>44</v>
+      </c>
+      <c r="B11" s="64">
         <v>100</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="68">
+        <v>61</v>
+      </c>
+      <c r="E11" s="65">
         <f>B11*1000</f>
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="64">
+        <v>10</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="67">
-        <v>10</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="D12" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="68">
+        <v>62</v>
+      </c>
+      <c r="E12" s="65">
         <f>B12*1000</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="67">
+        <v>46</v>
+      </c>
+      <c r="B13" s="64">
         <v>1737.4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="68">
+        <v>63</v>
+      </c>
+      <c r="E13" s="65">
         <f>B13*1000</f>
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="67">
+        <v>47</v>
+      </c>
+      <c r="B14" s="64">
         <v>1737.4</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="68">
+        <v>64</v>
+      </c>
+      <c r="E14" s="65">
         <f>B14*1000</f>
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="67">
+        <v>123</v>
+      </c>
+      <c r="B15" s="64">
         <v>13.17635815</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="68">
+        <v>65</v>
+      </c>
+      <c r="E15" s="65">
         <f>RADIANS(B15)/86400</f>
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="67">
+        <v>48</v>
+      </c>
+      <c r="B16" s="64">
         <v>0</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="68">
+        <v>66</v>
+      </c>
+      <c r="E16" s="65">
         <f>B16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="67">
+        <v>49</v>
+      </c>
+      <c r="B17" s="64">
         <v>0</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="68">
+        <v>67</v>
+      </c>
+      <c r="E17" s="65">
         <f>B17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="67">
+        <v>50</v>
+      </c>
+      <c r="B18" s="64">
         <v>0</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="68">
+        <v>68</v>
+      </c>
+      <c r="E18" s="65">
         <f>B18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="71">
+        <v>242</v>
+      </c>
+      <c r="B19" s="68">
         <f>$B$5/2</f>
         <v>3404.7101009954345</v>
       </c>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="68">
+        <v>243</v>
+      </c>
+      <c r="E19" s="65">
         <f t="shared" ref="E19:E21" si="1">B19</f>
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="71">
+        <v>127</v>
+      </c>
+      <c r="B20" s="68">
         <f>$B$5/2</f>
         <v>3404.7101009954345</v>
       </c>
-      <c r="C20" s="70" t="s">
+      <c r="C20" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="68">
+        <v>69</v>
+      </c>
+      <c r="E20" s="65">
         <f t="shared" si="1"/>
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" s="71">
+        <v>128</v>
+      </c>
+      <c r="B21" s="68">
         <f>$B$5/2</f>
         <v>3404.7101009954345</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="68">
+        <v>70</v>
+      </c>
+      <c r="E21" s="65">
         <f t="shared" si="1"/>
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="69">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="B22" s="66">
+        <v>1</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="68">
+        <v>35</v>
+      </c>
+      <c r="E22" s="65">
         <f t="shared" ref="E22:E24" si="2">B22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="69">
+      <c r="B23" s="66">
         <v>0</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -1688,351 +1882,582 @@
       <c r="D23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="69">
+        <v>36</v>
+      </c>
+      <c r="B24" s="66">
         <v>0</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="68">
+        <v>37</v>
+      </c>
+      <c r="E24" s="65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" s="67">
+        <v>147</v>
+      </c>
+      <c r="B25" s="64">
         <v>0</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="68">
+        <v>148</v>
+      </c>
+      <c r="E25" s="65">
         <f t="shared" ref="E25:E30" si="3">RADIANS(B25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26" s="67">
+        <v>146</v>
+      </c>
+      <c r="B26" s="64">
         <v>0</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" s="68">
+        <v>149</v>
+      </c>
+      <c r="E26" s="65">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B27" s="67">
+        <v>145</v>
+      </c>
+      <c r="B27" s="64">
         <v>180</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="68">
+        <v>150</v>
+      </c>
+      <c r="E27" s="65">
         <f t="shared" si="3"/>
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B28" s="67">
+        <v>151</v>
+      </c>
+      <c r="B28" s="64">
         <v>0</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E28" s="68">
+        <v>154</v>
+      </c>
+      <c r="E28" s="65">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="B29" s="67">
+        <v>152</v>
+      </c>
+      <c r="B29" s="64">
         <v>10</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="E29" s="68">
+        <v>155</v>
+      </c>
+      <c r="E29" s="65">
         <f t="shared" si="3"/>
         <v>0.17453292519943295</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="B30" s="67">
+        <v>153</v>
+      </c>
+      <c r="B30" s="64">
         <v>0</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E30" s="68">
+        <v>156</v>
+      </c>
+      <c r="E30" s="65">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B31" s="67">
+        <v>142</v>
+      </c>
+      <c r="B31" s="64">
         <v>30</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E31" s="68">
+        <v>174</v>
+      </c>
+      <c r="E31" s="65">
         <f t="shared" ref="E31:E32" si="4">B31</f>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="67">
+        <v>144</v>
+      </c>
+      <c r="B32" s="64">
         <v>0</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" s="68">
+        <v>173</v>
+      </c>
+      <c r="E32" s="65">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B33" s="67">
+        <v>164</v>
+      </c>
+      <c r="B33" s="64">
         <v>19</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="68">
+        <v>169</v>
+      </c>
+      <c r="E33" s="65">
         <f>B33/1000</f>
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" s="67">
+        <v>175</v>
+      </c>
+      <c r="B34" s="64">
         <v>7</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="68">
+        <v>170</v>
+      </c>
+      <c r="E34" s="65">
         <f>B34*0.000001</f>
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35" s="67">
+        <v>167</v>
+      </c>
+      <c r="B35" s="64">
         <v>2500</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="E35" s="68">
+        <v>171</v>
+      </c>
+      <c r="E35" s="65">
         <f t="shared" ref="E35:E36" si="5">B35</f>
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B36" s="67">
+        <v>168</v>
+      </c>
+      <c r="B36" s="64">
         <v>2500</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="68">
+        <v>172</v>
+      </c>
+      <c r="E36" s="65">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="B37" s="69">
+        <v>176</v>
+      </c>
+      <c r="B37" s="66">
         <v>5</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E37" s="68">
+        <v>177</v>
+      </c>
+      <c r="E37" s="65">
         <f>B37</f>
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" s="54">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="51">
         <v>1</v>
       </c>
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="E38" s="56">
+      <c r="D38" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="53">
         <f t="shared" ref="E38:E40" si="6">B38</f>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="B39" s="58">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="55">
         <v>1</v>
       </c>
-      <c r="C39" s="59" t="s">
+      <c r="C39" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="59" t="s">
-        <v>163</v>
-      </c>
-      <c r="E39" s="60">
+      <c r="D39" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" s="57">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
-        <v>206</v>
-      </c>
-      <c r="B40" s="74">
-        <v>0</v>
-      </c>
-      <c r="C40" s="52" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40" s="71">
+        <v>0</v>
+      </c>
+      <c r="C40" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="52" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" s="66">
+      <c r="D40" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="63">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="B41" s="69">
+        <v>180</v>
+      </c>
+      <c r="B41" s="66">
         <v>0</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41" s="68">
+        <v>181</v>
+      </c>
+      <c r="E41" s="65">
         <f t="shared" ref="E41" si="7">B41</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="72">
+        <v>182</v>
+      </c>
+      <c r="B42" s="69">
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="E42" s="73">
-        <f t="shared" ref="E42" si="8">B42</f>
-        <v>0</v>
+        <v>183</v>
+      </c>
+      <c r="E42" s="70">
+        <f t="shared" ref="E42:E55" si="8">B42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B43" s="66">
+        <v>3303</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="E43" s="83">
+        <f t="shared" si="8"/>
+        <v>3303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1.6242000000000001</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="8"/>
+        <v>1.6242000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1.6242000000000001</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" ref="E48" si="9">B48</f>
+        <v>1.6242000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" ref="E51" si="10">B51</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="B52" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B53" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" ref="E53:E54" si="11">B53</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="B54" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2047,12 +2472,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2060,7 +2485,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2068,7 +2493,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2077,7 +2502,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2085,9 +2510,9 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2100,25 +2525,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="73" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="23" t="s">
@@ -2128,169 +2554,458 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="30">
+        <v>-390</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="31">
+        <f t="shared" ref="E2:E4" si="0">B2*1000</f>
+        <v>-390000</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="33">
+        <v>10.3957</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="31">
+        <f t="shared" si="0"/>
+        <v>10395.699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="35">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="33">
+        <v>1700</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="31">
+        <f t="shared" ref="E5:E27" si="1">B5*1000</f>
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="31">
-        <v>1575.5547637675199</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="32">
-        <f t="shared" ref="E2:E4" si="0">B2*1000</f>
-        <v>1575554.76376752</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="34">
-        <v>-178.75415266497299</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="32">
-        <f t="shared" si="0"/>
-        <v>-178754.15266497299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="36">
-        <v>-928.32402032916605</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="37">
-        <f t="shared" si="0"/>
-        <v>-928324.02032916609</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="34">
-        <v>-0.50450806110878699</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="32">
-        <f>B5*1000</f>
-        <v>-504.50806110878699</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="34">
-        <v>-1.4165222911672899</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="32">
-        <f>B6*1000</f>
-        <v>-1416.5222911672899</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="34">
+      <c r="B7" s="33">
         <v>-0.58329957806655397</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="32">
-        <f>B7*1000</f>
+      <c r="C7" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="31">
+        <f t="shared" si="1"/>
         <v>-583.29957806655398</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="49">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="81" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="27">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>154</v>
+        <v>233</v>
       </c>
       <c r="E8" s="12">
-        <f>RADIANS(B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" s="29">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>155</v>
+        <v>234</v>
       </c>
       <c r="E9" s="13">
-        <f>RADIANS(B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="50">
-        <v>180</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" s="14">
-        <f>RADIANS(B10)</f>
-        <v>3.1415926535897931</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="27">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="80" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="74">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="75">
+        <v>0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="75">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="74">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="75">
+        <v>1737</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" s="65">
+        <f t="shared" si="1"/>
+        <v>1737000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="75">
+        <v>0</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="74">
+        <v>0</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="74">
+        <v>0</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E23" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="75">
+        <v>0</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="75">
+        <v>0</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" s="74">
+        <v>0</v>
+      </c>
+      <c r="C26" s="77" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E26" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="E27" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2301,39 +3016,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C720B3-BEEA-4D2E-BE7C-7EC9578AFA75}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2348,9 +3063,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2365,9 +3080,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -2382,15 +3097,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>207</v>
       </c>
       <c r="B5">
         <v>11</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -2399,80 +3114,125 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>208</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>13</v>
       </c>
       <c r="E6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8">
         <v>17</v>
       </c>
-      <c r="C7">
+      <c r="E8">
         <v>19</v>
       </c>
-      <c r="D7">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="C8">
-        <f>C4</f>
-        <v>10</v>
-      </c>
-      <c r="D8">
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
         <f>D2</f>
         <v>1</v>
       </c>
-      <c r="E8">
-        <f>E4</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9">
-        <f>B5</f>
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <f>C7</f>
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <f>D5</f>
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <f>E7</f>
-        <v>18</v>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2484,35 +3244,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD82E9-FB96-4FE4-9B12-1EDF4DE7082A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2527,9 +3289,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2544,114 +3306,110 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>208</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6">
+      <c r="C7">
         <v>14</v>
       </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>19</v>
-      </c>
       <c r="D7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <f>B2</f>
         <v>1</v>
       </c>
       <c r="C8">
-        <f>C4</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <f>D2</f>
         <v>1</v>
       </c>
       <c r="E8">
-        <f>E4</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <f>B5</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <f>C7</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <f>D5</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <f>E7</f>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2665,53 +3423,53 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="B2" s="26">
         <f>0.00000016*3</f>
         <v>4.8000000000000006E-7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="E2" s="13">
         <f>B2/3</f>
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -2730,7 +3488,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2748,135 +3506,135 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B5" s="10">
         <v>20</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E5" s="13">
         <f>RADIANS(B5)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B6" s="10">
         <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E6" s="13">
         <f>RADIANS(B6)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B7" s="10">
         <v>1.5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E7" s="13">
         <f>RADIANS(B7)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B8" s="10">
         <v>1.5</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B9" s="10">
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
-        <v>165</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
+        <v>138</v>
       </c>
       <c r="B10" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>168</v>
+      <c r="C10" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="E10" s="12">
         <f>B10/3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="B11" s="20">
         <v>3</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="E11" s="14">
         <f>B11/3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="B12" s="9">
         <v>10</v>
@@ -2885,16 +3643,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="E12" s="1">
         <f>B12/3</f>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="B13" s="9">
         <v>100</v>
@@ -2903,16 +3661,16 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="E13" s="1">
         <f>B13/3</f>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="B14" s="9">
         <v>10</v>
@@ -2921,7 +3679,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="E14" s="1">
         <f>B14/3</f>
@@ -2942,17 +3700,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2966,12 +3724,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4">
         <v>4000</v>
@@ -2980,16 +3738,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E2" s="12">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B3" s="6">
         <v>4000</v>
@@ -2998,16 +3756,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E3" s="13">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B4" s="6">
         <v>4000</v>
@@ -3016,70 +3774,70 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B8" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3088,16 +3846,16 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B9" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3106,16 +3864,16 @@
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B10" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3124,130 +3882,130 @@
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B11" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E11" s="13">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B12" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E12" s="13">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B13" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B14" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B15" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E15" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B16" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E16" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B17" s="6">
         <f>truthStateParams!$B$3</f>
@@ -3257,16 +4015,16 @@
         <v>25</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E17" s="13">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B18" s="6">
         <f>truthStateParams!$B$3</f>
@@ -3276,16 +4034,16 @@
         <v>25</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E18" s="13">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B19" s="8">
         <f>truthStateParams!$B$3</f>
@@ -3295,7 +4053,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E19" s="14">
         <f>RADIANS(B19)/hr2sec/3</f>
@@ -3314,35 +4072,35 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -3365,7 +4123,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -3388,7 +4146,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -3411,7 +4169,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -3434,7 +4192,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -3456,7 +4214,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -3478,7 +4236,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -3500,7 +4258,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -3522,8 +4280,8 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="str">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
@@ -3531,11 +4289,11 @@
         <f>truthStateParams!B10</f>
         <v>3</v>
       </c>
-      <c r="C10" s="52" t="str">
+      <c r="C10" s="49" t="str">
         <f>truthStateParams!C10</f>
         <v>pixels</v>
       </c>
-      <c r="D10" s="52" t="str">
+      <c r="D10" s="49" t="str">
         <f>truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
@@ -3544,7 +4302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -3566,7 +4324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -3588,7 +4346,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -3610,7 +4368,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -3646,34 +4404,34 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -3690,13 +4448,13 @@
         <f>truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="42">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -3713,13 +4471,13 @@
         <f>truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="42">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -3736,13 +4494,13 @@
         <f>truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="42">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -3759,13 +4517,13 @@
         <f>truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -3782,12 +4540,12 @@
         <f>truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -3804,12 +4562,12 @@
         <f>truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -3826,12 +4584,12 @@
         <f>truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="42">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -3848,12 +4606,12 @@
         <f>truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="42">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -3870,12 +4628,12 @@
         <f>truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="42">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -3892,12 +4650,12 @@
         <f>truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="42">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -3914,12 +4672,12 @@
         <f>truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="42">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -3936,12 +4694,12 @@
         <f>truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="42">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -3958,12 +4716,12 @@
         <f>truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="42">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -3980,12 +4738,12 @@
         <f>truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4002,12 +4760,12 @@
         <f>truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="42">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4024,12 +4782,12 @@
         <f>truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="42">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4046,12 +4804,12 @@
         <f>truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="42">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4068,7 +4826,7 @@
         <f>truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="43">
         <f>RADIANS(B19)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4081,40 +4839,40 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B2" s="6">
         <v>100</v>
@@ -4124,17 +4882,17 @@
         <v>m</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="43">
+        <v>129</v>
+      </c>
+      <c r="E2" s="42">
         <f t="shared" ref="E2:E7" si="0">B2</f>
         <v>100</v>
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B3" s="6">
         <v>200</v>
@@ -4144,27 +4902,27 @@
         <v>m</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="43">
+        <v>129</v>
+      </c>
+      <c r="E3" s="42">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="8">
         <v>300</v>
       </c>
-      <c r="C4" s="6" t="str">
+      <c r="C4" s="8" t="str">
         <f>truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>147</v>
+      <c r="D4" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" si="0"/>
@@ -4172,9 +4930,9 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -4184,17 +4942,17 @@
         <v>m/sec</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="43">
+        <v>130</v>
+      </c>
+      <c r="E5" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -4204,27 +4962,27 @@
         <v>m/sec</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="43">
+        <v>130</v>
+      </c>
+      <c r="E6" s="42">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="8">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="8" t="str">
         <f>truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>148</v>
+      <c r="D7" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="E7" s="43">
         <f t="shared" si="0"/>
@@ -4232,242 +4990,197 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="78" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="76">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="43">
+      <c r="C8" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="79">
         <f>B8/1000</f>
         <v>1E-3</v>
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>133</v>
+        <v>213</v>
       </c>
       <c r="B9" s="6">
         <v>2</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="43">
+        <v>221</v>
+      </c>
+      <c r="E9" s="42">
         <f>B9/1000</f>
         <v>2E-3</v>
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>134</v>
+        <v>214</v>
       </c>
       <c r="B10" s="6">
         <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="43">
+        <v>221</v>
+      </c>
+      <c r="E10" s="42">
         <f>B10/1000</f>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="8">
         <v>180</v>
       </c>
-      <c r="C11" s="6" t="str">
-        <f>truthStateInitialUncertainty!C11</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="43">
+        <f t="shared" ref="E11:E15" si="1">RADIANS(B11)/3600</f>
+        <v>8.726646259971648E-4</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="76">
         <v>150</v>
       </c>
-      <c r="E11" s="43">
-        <f t="shared" ref="E11:E16" si="1">RADIANS(B11)/3600</f>
-        <v>8.726646259971648E-4</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="6">
-        <v>150</v>
-      </c>
-      <c r="C12" s="6" t="str">
-        <f>truthStateInitialUncertainty!C12</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" s="43">
+      <c r="C12" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="79">
         <f t="shared" si="1"/>
         <v>7.2722052166430398E-4</v>
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="B13" s="6">
-        <v>130</v>
-      </c>
-      <c r="C13" s="6" t="str">
-        <f>truthStateInitialUncertainty!C13</f>
-        <v>arcsec</v>
+        <v>0.01</v>
+      </c>
+      <c r="C13" s="72" t="s">
+        <v>202</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13" s="43">
+        <v>223</v>
+      </c>
+      <c r="E13" s="42">
         <f t="shared" si="1"/>
-        <v>6.3025778544239684E-4</v>
+        <v>4.8481368110953601E-8</v>
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="B14" s="6">
-        <v>180</v>
-      </c>
-      <c r="C14" s="6" t="str">
-        <f>truthStateInitialUncertainty!C14</f>
-        <v>arcsec</v>
+        <v>0.02</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>202</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="43">
+        <v>223</v>
+      </c>
+      <c r="E14" s="42">
         <f t="shared" si="1"/>
-        <v>8.726646259971648E-4</v>
+        <v>9.6962736221907202E-8</v>
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="6">
-        <v>150</v>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>truthStateInitialUncertainty!C15</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>151</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="C15" s="77" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>223</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" si="1"/>
-        <v>7.2722052166430398E-4</v>
+        <v>1.4544410433286078E-7</v>
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="6">
-        <v>130</v>
-      </c>
-      <c r="C16" s="6" t="str">
-        <f>truthStateInitialUncertainty!C16</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="43">
-        <f t="shared" si="1"/>
-        <v>6.3025778544239684E-4</v>
-      </c>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="str">
-        <f>truthStateInitialUncertainty!C17</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="43">
-        <f>RADIANS(B17)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
-      </c>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>truthStateInitialUncertainty!C18</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="43">
-        <f>RADIANS(B18)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
-      </c>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8" t="str">
-        <f>truthStateInitialUncertainty!C19</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="44">
-        <f>RADIANS(B19)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
-      </c>
-      <c r="F19" s="8"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented the guidance law
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\epitts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47438A5-1E2B-0147-A0E0-5A27D56F6CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B19CF31-97A7-4C25-99E7-FC69C49CF77C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="465" windowWidth="16800" windowHeight="18915" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,6 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1454,21 +1444,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1475,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1511,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
@@ -1540,7 +1530,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
@@ -1559,7 +1549,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1577,7 +1567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
@@ -1595,7 +1585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>131</v>
       </c>
@@ -1614,7 +1604,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
@@ -1632,7 +1622,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
@@ -1650,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
@@ -1668,7 +1658,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>45</v>
       </c>
@@ -1686,7 +1676,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1704,7 +1694,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1722,7 +1712,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>123</v>
       </c>
@@ -1740,7 +1730,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>48</v>
       </c>
@@ -1758,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
@@ -1776,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>50</v>
       </c>
@@ -1794,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>242</v>
       </c>
@@ -1813,7 +1803,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>127</v>
       </c>
@@ -1832,7 +1822,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>128</v>
       </c>
@@ -1851,7 +1841,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>34</v>
       </c>
@@ -1869,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>20</v>
       </c>
@@ -1887,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>36</v>
       </c>
@@ -1905,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>147</v>
       </c>
@@ -1923,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>146</v>
       </c>
@@ -1941,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>145</v>
       </c>
@@ -1959,7 +1949,7 @@
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>151</v>
       </c>
@@ -1977,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>152</v>
       </c>
@@ -1995,7 +1985,7 @@
         <v>0.17453292519943295</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>153</v>
       </c>
@@ -2013,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>142</v>
       </c>
@@ -2031,7 +2021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>144</v>
       </c>
@@ -2049,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>164</v>
       </c>
@@ -2067,7 +2057,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>175</v>
       </c>
@@ -2085,7 +2075,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>167</v>
       </c>
@@ -2103,7 +2093,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>168</v>
       </c>
@@ -2121,7 +2111,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>176</v>
       </c>
@@ -2139,7 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
         <v>125</v>
       </c>
@@ -2157,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="54" t="s">
         <v>126</v>
       </c>
@@ -2175,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
         <v>179</v>
       </c>
@@ -2193,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>180</v>
       </c>
@@ -2211,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>182</v>
       </c>
@@ -2229,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>260</v>
       </c>
@@ -2247,7 +2237,7 @@
         <v>3303</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>244</v>
       </c>
@@ -2265,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>245</v>
       </c>
@@ -2283,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>247</v>
       </c>
@@ -2301,12 +2291,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>249</v>
       </c>
       <c r="B47" s="2">
-        <v>1.6242000000000001</v>
+        <v>1.62</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>202</v>
@@ -2316,15 +2306,15 @@
       </c>
       <c r="E47" s="1">
         <f t="shared" si="8"/>
-        <v>1.6242000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>264</v>
       </c>
       <c r="B48" s="2">
-        <v>1.6242000000000001</v>
+        <v>0</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>202</v>
@@ -2334,10 +2324,10 @@
       </c>
       <c r="E48" s="1">
         <f t="shared" ref="E48" si="9">B48</f>
-        <v>1.6242000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>251</v>
       </c>
@@ -2355,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>253</v>
       </c>
@@ -2373,12 +2363,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>265</v>
       </c>
       <c r="B51" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>254</v>
@@ -2388,15 +2378,15 @@
       </c>
       <c r="E51" s="1">
         <f t="shared" ref="E51" si="10">B51</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>256</v>
       </c>
       <c r="B52" s="2">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>8</v>
@@ -2406,15 +2396,15 @@
       </c>
       <c r="E52" s="1">
         <f t="shared" si="8"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>266</v>
       </c>
       <c r="B53" s="2">
-        <v>-2</v>
+        <v>1738</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>8</v>
@@ -2424,15 +2414,15 @@
       </c>
       <c r="E53" s="1">
         <f t="shared" ref="E53:E54" si="11">B53</f>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>267</v>
       </c>
       <c r="B54" s="2">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>8</v>
@@ -2442,10 +2432,10 @@
       </c>
       <c r="E54" s="1">
         <f t="shared" si="11"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>262</v>
       </c>
@@ -2472,12 +2462,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2485,7 +2475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2493,7 +2483,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2502,7 +2492,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2510,7 +2500,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -2527,20 +2517,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2557,7 +2547,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>72</v>
       </c>
@@ -2576,12 +2566,13 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="33">
-        <v>10.3957</v>
+        <f>10.3957+1737.5</f>
+        <v>1747.8957</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>52</v>
@@ -2591,10 +2582,10 @@
       </c>
       <c r="E3" s="31">
         <f t="shared" si="0"/>
-        <v>10395.699999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1747895.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>76</v>
       </c>
@@ -2612,12 +2603,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="33">
-        <v>1700</v>
+        <v>1.7</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>79</v>
@@ -2627,10 +2618,10 @@
       </c>
       <c r="E5" s="31">
         <f t="shared" ref="E5:E27" si="1">B5*1000</f>
-        <v>1700000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>80</v>
       </c>
@@ -2648,12 +2639,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="33">
-        <v>-0.58329957806655397</v>
+        <v>0</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>79</v>
@@ -2663,10 +2654,10 @@
       </c>
       <c r="E7" s="31">
         <f t="shared" si="1"/>
-        <v>-583.29957806655398</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="81" t="s">
         <v>225</v>
       </c>
@@ -2682,7 +2673,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>226</v>
       </c>
@@ -2698,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>227</v>
       </c>
@@ -2714,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
         <v>228</v>
       </c>
@@ -2730,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>229</v>
       </c>
@@ -2746,7 +2737,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>230</v>
       </c>
@@ -2761,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>231</v>
       </c>
@@ -2776,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="80" t="s">
         <v>232</v>
       </c>
@@ -2792,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
         <v>184</v>
       </c>
@@ -2810,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>185</v>
       </c>
@@ -2828,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
         <v>186</v>
       </c>
@@ -2846,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>187</v>
       </c>
@@ -2864,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>188</v>
       </c>
@@ -2882,7 +2873,7 @@
         <v>1737000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -2900,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>190</v>
       </c>
@@ -2918,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>191</v>
       </c>
@@ -2936,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -2954,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>193</v>
       </c>
@@ -2972,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>194</v>
       </c>
@@ -2990,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>258</v>
       </c>
@@ -3019,17 +3010,17 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3046,7 +3037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3063,7 +3054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3080,7 +3071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3097,7 +3088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -3114,7 +3105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -3131,7 +3122,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -3148,7 +3139,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -3165,7 +3156,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -3182,7 +3173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>210</v>
       </c>
@@ -3199,7 +3190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -3218,7 +3209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3248,14 +3239,14 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3272,7 +3263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3289,7 +3280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3306,7 +3297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -3323,7 +3314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -3340,7 +3331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -3357,7 +3348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -3374,7 +3365,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3393,7 +3384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3423,17 +3414,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -3450,7 +3441,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>132</v>
       </c>
@@ -3469,7 +3460,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -3488,7 +3479,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3506,7 +3497,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>103</v>
       </c>
@@ -3524,7 +3515,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>104</v>
       </c>
@@ -3542,7 +3533,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>105</v>
       </c>
@@ -3560,7 +3551,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>106</v>
       </c>
@@ -3578,7 +3569,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3596,7 +3587,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>138</v>
       </c>
@@ -3614,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>139</v>
       </c>
@@ -3632,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>157</v>
       </c>
@@ -3650,7 +3641,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>159</v>
       </c>
@@ -3668,7 +3659,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>161</v>
       </c>
@@ -3700,17 +3691,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3727,7 +3718,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -3745,7 +3736,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -3763,7 +3754,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
@@ -3781,7 +3772,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -3799,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>94</v>
       </c>
@@ -3817,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
@@ -3835,7 +3826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>108</v>
       </c>
@@ -3853,7 +3844,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>109</v>
       </c>
@@ -3871,7 +3862,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>110</v>
       </c>
@@ -3889,7 +3880,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>114</v>
       </c>
@@ -3908,7 +3899,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>115</v>
       </c>
@@ -3927,7 +3918,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>116</v>
       </c>
@@ -3946,7 +3937,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>111</v>
       </c>
@@ -3965,7 +3956,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>112</v>
       </c>
@@ -3984,7 +3975,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>113</v>
       </c>
@@ -4003,7 +3994,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>99</v>
       </c>
@@ -4022,7 +4013,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>101</v>
       </c>
@@ -4041,7 +4032,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>102</v>
       </c>
@@ -4072,18 +4063,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4100,7 +4091,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -4123,7 +4114,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -4146,7 +4137,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -4169,7 +4160,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -4192,7 +4183,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -4214,7 +4205,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -4236,7 +4227,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -4258,7 +4249,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -4280,7 +4271,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -4302,7 +4293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -4324,7 +4315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -4346,7 +4337,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -4368,7 +4359,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -4404,17 +4395,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4431,7 +4422,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -4454,7 +4445,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -4477,7 +4468,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -4500,7 +4491,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -4523,7 +4514,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -4545,7 +4536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -4567,7 +4558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4589,7 +4580,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4611,7 +4602,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4633,7 +4624,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4655,7 +4646,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4677,7 +4668,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4699,7 +4690,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4721,7 +4712,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4743,7 +4734,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4765,7 +4756,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4787,7 +4778,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4809,7 +4800,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4845,15 +4836,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4870,7 +4861,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>117</v>
       </c>
@@ -4890,7 +4881,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>118</v>
       </c>
@@ -4910,7 +4901,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>119</v>
       </c>
@@ -4930,7 +4921,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>120</v>
       </c>
@@ -4950,7 +4941,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>121</v>
       </c>
@@ -4970,7 +4961,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>122</v>
       </c>
@@ -4990,7 +4981,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
         <v>212</v>
       </c>
@@ -5009,7 +5000,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>213</v>
       </c>
@@ -5028,7 +5019,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>214</v>
       </c>
@@ -5047,7 +5038,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>215</v>
       </c>
@@ -5066,7 +5057,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
         <v>216</v>
       </c>
@@ -5085,7 +5076,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>217</v>
       </c>
@@ -5104,7 +5095,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>218</v>
       </c>
@@ -5123,7 +5114,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>219</v>
       </c>
@@ -5142,7 +5133,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5150,7 +5141,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5158,7 +5149,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5166,7 +5157,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5174,7 +5165,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>

</xml_diff>

<commit_message>
Modifying truthState_de and config
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\epitts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B19CF31-97A7-4C25-99E7-FC69C49CF77C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA13794-5FD2-E846-B95D-9C0138432F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="465" windowWidth="16800" windowHeight="18915" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,21 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="273">
   <si>
     <t>Value</t>
   </si>
@@ -248,9 +258,6 @@
     <t>Star camera misalignment ECRV time constant</t>
   </si>
   <si>
-    <t>Terrain camera misalignment ECRV time constant</t>
-  </si>
-  <si>
     <t>gbias</t>
   </si>
   <si>
@@ -419,12 +426,6 @@
     <t>processVisualOdometryEnable</t>
   </si>
   <si>
-    <t>tau_st</t>
-  </si>
-  <si>
-    <t>tau_c</t>
-  </si>
-  <si>
     <t>Injected satellite position error</t>
   </si>
   <si>
@@ -818,18 +819,6 @@
     <t>Downrange location of landing site</t>
   </si>
   <si>
-    <t>tau_ax</t>
-  </si>
-  <si>
-    <t>Acceleration bias</t>
-  </si>
-  <si>
-    <t>seed_h</t>
-  </si>
-  <si>
-    <t>Seed for the terrain generator</t>
-  </si>
-  <si>
     <t>astar_z_tf</t>
   </si>
   <si>
@@ -840,6 +829,42 @@
   </si>
   <si>
     <t>rstar_z_tf</t>
+  </si>
+  <si>
+    <t>sig_grav_ss</t>
+  </si>
+  <si>
+    <t>Q_nongra</t>
+  </si>
+  <si>
+    <t>sig_lbias_ss</t>
+  </si>
+  <si>
+    <t>sig_lscale_ss</t>
+  </si>
+  <si>
+    <t>sig_abias_ss</t>
+  </si>
+  <si>
+    <t>tau_a</t>
+  </si>
+  <si>
+    <t>omega_moon</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>rad/s</t>
+  </si>
+  <si>
+    <t>Moon rotation rate</t>
+  </si>
+  <si>
+    <t>m3/s2</t>
+  </si>
+  <si>
+    <t>Moon gravitational constant</t>
   </si>
 </sst>
 </file>
@@ -852,7 +877,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -871,6 +896,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1019,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1103,7 +1135,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1444,21 +1477,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:B54"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
@@ -1472,10 +1505,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="61" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
@@ -1493,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1511,7 +1544,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
@@ -1530,7 +1563,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1582,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
@@ -1585,9 +1618,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B8" s="66">
         <f>12*6</f>
@@ -1604,7 +1637,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
@@ -1622,7 +1655,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
@@ -1640,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
@@ -1658,7 +1691,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>45</v>
       </c>
@@ -1676,7 +1709,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1694,7 +1727,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1712,9 +1745,9 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" s="64">
         <v>13.17635815</v>
@@ -1730,7 +1763,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>48</v>
       </c>
@@ -1748,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
@@ -1766,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>50</v>
       </c>
@@ -1784,9 +1817,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B19" s="68">
         <f>$B$5/2</f>
@@ -1796,16 +1829,16 @@
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E19" s="65">
-        <f t="shared" ref="E19:E21" si="1">B19</f>
+        <f t="shared" ref="E19:E20" si="1">B19</f>
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
       <c r="B20" s="68">
         <f>$B$5/2</f>
@@ -1822,46 +1855,45 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" s="68">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
-      </c>
-      <c r="C21" s="67" t="s">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="B21" s="66">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E21" s="65">
-        <f t="shared" si="1"/>
-        <v>3404.7101009954345</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E21:E23" si="2">B21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B22" s="66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E22" s="65">
-        <f t="shared" ref="E22:E24" si="2">B22</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B23" s="66">
         <v>0</v>
@@ -1870,34 +1902,34 @@
         <v>4</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E23" s="65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="66">
+        <v>144</v>
+      </c>
+      <c r="B24" s="64">
         <v>0</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="E24" s="65">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E24:E29" si="3">RADIANS(B24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B25" s="64">
         <v>0</v>
@@ -1906,549 +1938,539 @@
         <v>22</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E25" s="65">
-        <f t="shared" ref="E25:E30" si="3">RADIANS(B25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B26" s="64">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E26" s="65">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.1415926535897931</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B27" s="64">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E27" s="65">
         <f t="shared" si="3"/>
-        <v>3.1415926535897931</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B28" s="64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E28" s="65">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.17453292519943295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B29" s="64">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E29" s="65">
         <f t="shared" si="3"/>
-        <v>0.17453292519943295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B30" s="64">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="E30" s="65">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E30:E31" si="4">B30</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31" s="64">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>143</v>
+        <v>4</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E31" s="65">
-        <f t="shared" ref="E31:E32" si="4">B31</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="B32" s="64">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E32" s="65">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <f>B32/1000</f>
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="64">
+        <v>7</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="65">
+        <f>B33*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="B33" s="64">
-        <v>19</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="65">
-        <f>B33/1000</f>
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>175</v>
-      </c>
       <c r="B34" s="64">
-        <v>7</v>
+        <v>2500</v>
       </c>
       <c r="C34" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="65">
+        <f t="shared" ref="E34:E35" si="5">B34</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
         <v>165</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" s="65">
-        <f>B34*0.000001</f>
-        <v>6.9999999999999999E-6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>167</v>
       </c>
       <c r="B35" s="64">
         <v>2500</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E35" s="65">
-        <f t="shared" ref="E35:E36" si="5">B35</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="64">
-        <v>2500</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="65">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" s="66">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="66">
         <v>5</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C36" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="E37" s="65">
-        <f>B37</f>
+      <c r="D36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="65">
+        <f>B36</f>
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="51">
+        <v>1</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="53">
+        <f t="shared" ref="E37:E39" si="6">B37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="51">
+      <c r="B38" s="55">
         <v>1</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="53">
-        <f t="shared" ref="E38:E40" si="6">B38</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="55">
-        <v>1</v>
-      </c>
-      <c r="C39" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="E39" s="57">
+      <c r="D38" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="57">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" s="71">
+        <v>0</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" s="63">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="66">
+        <v>0</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="65">
+        <f t="shared" ref="E40" si="7">B40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B40" s="71">
-        <v>0</v>
-      </c>
-      <c r="C40" s="49" t="s">
+      <c r="B41" s="69">
+        <v>0</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="E40" s="63">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B41" s="66">
-        <v>0</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E41" s="65">
-        <f t="shared" ref="E41" si="7">B41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B42" s="69">
-        <v>0</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="E42" s="70">
-        <f t="shared" ref="E42:E55" si="8">B42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B43" s="66">
-        <v>3303</v>
+      <c r="E41" s="70">
+        <f t="shared" ref="E41:E55" si="8">B41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1737.5</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="8"/>
+        <v>1737.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1737.5</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="E43" s="83">
+        <v>243</v>
+      </c>
+      <c r="E43" s="1">
         <f t="shared" si="8"/>
-        <v>3303</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1737.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
         <v>244</v>
       </c>
       <c r="B44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B45" s="2">
-        <v>1</v>
+        <v>1.6242000000000001</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.6242000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.6242000000000001</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D46" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B46" s="2">
-        <v>0</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D46" s="16" t="s">
+      <c r="E46" s="1">
+        <f t="shared" ref="E46" si="9">B46</f>
+        <v>1.6242000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="E46" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>249</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1.62</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>250</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="8"/>
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B48" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>202</v>
+        <v>251</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" ref="E48" si="9">B48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>251</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>254</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>252</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E49" si="10">B49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>253</v>
       </c>
       <c r="B50" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>254</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>255</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B51" s="2">
-        <v>0</v>
+        <v>-1738</v>
       </c>
       <c r="C51" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="D51" s="16" t="s">
-        <v>255</v>
-      </c>
       <c r="E51" s="1">
-        <f t="shared" ref="E51" si="10">B51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E51:E54" si="11">B51</f>
+        <v>-1738</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B52" s="2">
         <v>0</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="B53" s="2">
-        <v>1738</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>257</v>
+        <v>267</v>
+      </c>
+      <c r="B53" s="83">
+        <v>2.7E-6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" t="s">
+        <v>270</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" ref="E53:E54" si="11">B53</f>
-        <v>1738</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>2.7E-6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="B54" s="2">
-        <v>0</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>257</v>
+        <v>268</v>
+      </c>
+      <c r="B54" s="84">
+        <v>4904869500000</v>
+      </c>
+      <c r="C54" t="s">
+        <v>271</v>
+      </c>
+      <c r="D54" t="s">
+        <v>272</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="B55" s="2">
-        <v>2</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="E55" s="1">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
+        <v>4904869500000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="18"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2460,14 +2482,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2475,7 +2499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2483,7 +2507,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2492,7 +2516,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2500,9 +2524,9 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2517,20 +2541,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2544,12 +2568,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="30">
         <v>-390</v>
@@ -2558,7 +2582,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="31">
         <f t="shared" ref="E2:E4" si="0">B2*1000</f>
@@ -2566,28 +2590,27 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="33">
-        <f>10.3957+1737.5</f>
-        <v>1747.8957</v>
+        <v>10.3957</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="31">
         <f t="shared" si="0"/>
-        <v>1747895.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10395.699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="35">
         <v>0</v>
@@ -2596,196 +2619,196 @@
         <v>52</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="33">
         <v>1.7</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="31">
         <f t="shared" ref="E5:E27" si="1">B5*1000</f>
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="33">
         <v>0</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="33">
-        <v>0</v>
+        <v>-0.58329957806655397</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-583.29957806655398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B8" s="27">
         <v>1</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E8" s="12">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B9" s="15">
         <v>0</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B10" s="15">
         <v>0</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B12" s="27">
         <v>1</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="49" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E12" s="12">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B13" s="15">
         <v>0</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B14" s="15">
         <v>0</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="80" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B15" s="20">
         <v>0</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E15" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="47" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B16" s="74">
         <v>0</v>
@@ -2794,70 +2817,70 @@
         <v>52</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E16" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B17" s="75">
         <v>0</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B18" s="75">
         <v>0</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B19" s="74">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E19" s="70">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B20" s="75">
         <v>1737</v>
@@ -2866,16 +2889,16 @@
         <v>52</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E20" s="65">
         <f t="shared" si="1"/>
         <v>1737000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B21" s="75">
         <v>0</v>
@@ -2884,16 +2907,16 @@
         <v>52</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E21" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B22" s="74">
         <v>0</v>
@@ -2902,16 +2925,16 @@
         <v>52</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E22" s="70">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B23" s="74">
         <v>0</v>
@@ -2920,70 +2943,70 @@
         <v>52</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E23" s="70">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B24" s="75">
         <v>0</v>
       </c>
       <c r="C24" s="72" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E24" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B25" s="75">
         <v>0</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E25" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B26" s="74">
         <v>0</v>
       </c>
       <c r="C26" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>205</v>
       </c>
       <c r="E26" s="70">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B27" s="9">
         <v>0</v>
@@ -2992,7 +3015,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E27" s="65">
         <f t="shared" si="1"/>
@@ -3010,17 +3033,17 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3037,7 +3060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3054,7 +3077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3071,9 +3094,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3088,9 +3111,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -3105,9 +3128,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -3122,9 +3145,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -3139,9 +3162,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -3156,9 +3179,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B9">
         <v>22</v>
@@ -3173,9 +3196,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B10">
         <v>23</v>
@@ -3190,7 +3213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -3209,7 +3232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3239,14 +3262,14 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3280,7 +3303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3297,9 +3320,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3314,9 +3337,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -3331,9 +3354,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -3348,9 +3371,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3365,7 +3388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3384,7 +3407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3410,21 +3433,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -3438,29 +3463,29 @@
         <v>1</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B2" s="26">
         <f>0.00000016*3</f>
         <v>4.8000000000000006E-7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" s="13">
         <f>B2/3</f>
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -3479,7 +3504,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3497,135 +3522,135 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="10">
         <v>20</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>83</v>
       </c>
       <c r="E5" s="13">
         <f>RADIANS(B5)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="10">
         <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="13">
         <f>RADIANS(B6)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="10">
         <v>1.5</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="E7" s="13">
         <f>RADIANS(B7)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="10">
         <v>1.5</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="10">
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" s="27">
         <v>3</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E10" s="12">
-        <f>B10/3</f>
+        <f t="shared" ref="E10:E15" si="1">B10/3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" s="20">
         <v>3</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="E11" s="14">
-        <f>B11/3</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B12" s="9">
         <v>10</v>
@@ -3634,16 +3659,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E12" s="1">
-        <f>B12/3</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B13" s="9">
         <v>100</v>
@@ -3652,16 +3677,16 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E13" s="1">
-        <f>B13/3</f>
+        <f t="shared" si="1"/>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B14" s="9">
         <v>10</v>
@@ -3670,11 +3695,62 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E14" s="1">
-        <f>B14/3</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="9">
+        <v>5</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" s="26">
+        <f>0.00000016*3</f>
+        <v>4.8000000000000006E-7</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3691,17 +3767,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3715,12 +3791,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="4">
         <v>4000</v>
@@ -3729,16 +3805,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="12">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="6">
         <v>4000</v>
@@ -3747,16 +3823,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="13">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="6">
         <v>4000</v>
@@ -3765,70 +3841,70 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3837,16 +3913,16 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3855,16 +3931,16 @@
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6">
         <v>5.0000000000000001E-4</v>
@@ -3873,130 +3949,130 @@
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="13">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="13">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="6">
         <f>truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" s="6">
         <f>truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="13">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="6">
         <f>truthStateParams!$B$3</f>
@@ -4006,16 +4082,16 @@
         <v>25</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E17" s="13">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="6">
         <f>truthStateParams!$B$3</f>
@@ -4025,16 +4101,16 @@
         <v>25</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E18" s="13">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="8">
         <f>truthStateParams!$B$3</f>
@@ -4044,7 +4120,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E19" s="14">
         <f>RADIANS(B19)/hr2sec/3</f>
@@ -4063,18 +4139,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4088,10 +4164,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -4114,7 +4190,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -4137,7 +4213,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -4160,7 +4236,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -4183,7 +4259,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -4205,7 +4281,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -4227,7 +4303,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -4249,7 +4325,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -4271,7 +4347,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -4293,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -4315,7 +4391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -4337,7 +4413,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -4359,7 +4435,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -4395,17 +4471,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4419,10 +4495,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -4445,7 +4521,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -4468,7 +4544,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -4491,7 +4567,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -4514,7 +4590,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -4536,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -4558,7 +4634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4580,7 +4656,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4602,7 +4678,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4624,7 +4700,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4646,7 +4722,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4668,7 +4744,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4690,7 +4766,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4712,7 +4788,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4734,7 +4810,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4756,7 +4832,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4778,7 +4854,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4800,7 +4876,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4836,15 +4912,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4858,12 +4934,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="6">
         <v>100</v>
@@ -4873,7 +4949,7 @@
         <v>m</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E2" s="42">
         <f t="shared" ref="E2:E7" si="0">B2</f>
@@ -4881,9 +4957,9 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="6">
         <v>200</v>
@@ -4893,7 +4969,7 @@
         <v>m</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E3" s="42">
         <f t="shared" si="0"/>
@@ -4901,9 +4977,9 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="8">
         <v>300</v>
@@ -4913,7 +4989,7 @@
         <v>m</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" si="0"/>
@@ -4921,9 +4997,9 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -4933,7 +5009,7 @@
         <v>m/sec</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E5" s="42">
         <f t="shared" si="0"/>
@@ -4941,9 +5017,9 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -4953,7 +5029,7 @@
         <v>m/sec</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E6" s="42">
         <f t="shared" si="0"/>
@@ -4961,9 +5037,9 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8">
         <v>3</v>
@@ -4973,7 +5049,7 @@
         <v>m/sec</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E7" s="43">
         <f t="shared" si="0"/>
@@ -4981,9 +5057,9 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B8" s="76">
         <v>1</v>
@@ -4992,7 +5068,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="76" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E8" s="79">
         <f>B8/1000</f>
@@ -5000,18 +5076,18 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B9" s="6">
         <v>2</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E9" s="42">
         <f>B9/1000</f>
@@ -5019,18 +5095,18 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B10" s="6">
         <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E10" s="42">
         <f>B10/1000</f>
@@ -5038,18 +5114,18 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B11" s="8">
         <v>180</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E11" s="43">
         <f t="shared" ref="E11:E15" si="1">RADIANS(B11)/3600</f>
@@ -5057,9 +5133,9 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="78" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B12" s="76">
         <v>150</v>
@@ -5068,7 +5144,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="76" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E12" s="79">
         <f t="shared" si="1"/>
@@ -5076,18 +5152,18 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B13" s="6">
         <v>0.01</v>
       </c>
       <c r="C13" s="72" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E13" s="42">
         <f t="shared" si="1"/>
@@ -5095,18 +5171,18 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B14" s="6">
         <v>0.02</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E14" s="42">
         <f t="shared" si="1"/>
@@ -5114,18 +5190,18 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B15" s="8">
         <v>0.03</v>
       </c>
       <c r="C15" s="77" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" si="1"/>
@@ -5133,7 +5209,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5141,7 +5217,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5149,7 +5225,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5157,7 +5233,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5165,7 +5241,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>

</xml_diff>

<commit_message>
Removing state, changing some config values, debugging various functions, correcting typo in main, adding position plot, relocating loss functions
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA13794-5FD2-E846-B95D-9C0138432F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E571A1B-016B-8C4D-8E0B-3BD376D7F2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="263">
   <si>
     <t>Value</t>
   </si>
@@ -603,15 +603,6 @@
     <t>epsilong_z</t>
   </si>
   <si>
-    <t>rf_x</t>
-  </si>
-  <si>
-    <t>rf_y</t>
-  </si>
-  <si>
-    <t>rf_z</t>
-  </si>
-  <si>
     <t>h_t</t>
   </si>
   <si>
@@ -633,15 +624,6 @@
     <t>z component of bias in gravity of the moon</t>
   </si>
   <si>
-    <t>x component of the position of the observed feature</t>
-  </si>
-  <si>
-    <t>y component of the position of the observed feature</t>
-  </si>
-  <si>
-    <t>z component of the position of the observed feature</t>
-  </si>
-  <si>
     <t>clock bias, seen as bias in the measured range</t>
   </si>
   <si>
@@ -666,15 +648,9 @@
     <t>b_clock</t>
   </si>
   <si>
-    <t>pos_f</t>
-  </si>
-  <si>
     <t>b_accl</t>
   </si>
   <si>
-    <t>b_accel</t>
-  </si>
-  <si>
     <t>del_b</t>
   </si>
   <si>
@@ -811,12 +787,6 @@
   </si>
   <si>
     <t>Desired downrange position at final time</t>
-  </si>
-  <si>
-    <t>r0</t>
-  </si>
-  <si>
-    <t>Downrange location of landing site</t>
   </si>
   <si>
     <t>astar_z_tf</t>
@@ -1051,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1134,7 +1104,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -1477,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1819,7 +1788,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B19" s="68">
         <f>$B$5/2</f>
@@ -1829,7 +1798,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E19" s="65">
         <f t="shared" ref="E19:E20" si="1">B19</f>
@@ -1838,7 +1807,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B20" s="68">
         <f>$B$5/2</f>
@@ -2229,13 +2198,13 @@
         <v>180</v>
       </c>
       <c r="E41" s="70">
-        <f t="shared" ref="E41:E55" si="8">B41</f>
+        <f t="shared" ref="E41:E50" si="8">B41</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B42" s="2">
         <v>1737.5</v>
@@ -2244,7 +2213,7 @@
         <v>52</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="8"/>
@@ -2253,7 +2222,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B43" s="2">
         <v>1737.5</v>
@@ -2262,7 +2231,7 @@
         <v>52</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="8"/>
@@ -2271,16 +2240,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B44" s="2">
         <v>0</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="8"/>
@@ -2289,16 +2258,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B45" s="2">
         <v>1.6242000000000001</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="8"/>
@@ -2307,16 +2276,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B46" s="2">
         <v>1.6242000000000001</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" ref="E46" si="9">B46</f>
@@ -2325,16 +2294,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B47" s="2">
         <v>0</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="8"/>
@@ -2343,16 +2312,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B48" s="2">
         <v>-1</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="8"/>
@@ -2361,16 +2330,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B49" s="2">
         <v>0</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" ref="E49" si="10">B49</f>
@@ -2379,7 +2348,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B50" s="2">
         <v>0</v>
@@ -2388,7 +2357,7 @@
         <v>52</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="8"/>
@@ -2397,7 +2366,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B51" s="2">
         <v>-1738</v>
@@ -2406,7 +2375,7 @@
         <v>52</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" ref="E51:E54" si="11">B51</f>
@@ -2415,7 +2384,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B52" s="2">
         <v>0</v>
@@ -2424,7 +2393,7 @@
         <v>52</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" si="11"/>
@@ -2433,16 +2402,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="B53" s="83">
+        <v>257</v>
+      </c>
+      <c r="B53" s="82">
         <v>2.7E-6</v>
       </c>
       <c r="C53" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D53" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="11"/>
@@ -2451,16 +2420,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="B54" s="84">
+        <v>258</v>
+      </c>
+      <c r="B54" s="83">
         <v>4904869500000</v>
       </c>
       <c r="C54" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D54" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="11"/>
@@ -2539,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2640,7 +2609,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="31">
-        <f t="shared" ref="E5:E27" si="1">B5*1000</f>
+        <f t="shared" ref="E5:E23" si="1">B5*1000</f>
         <v>1700</v>
       </c>
     </row>
@@ -2682,14 +2651,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B8" s="27">
         <v>1</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E8" s="12">
         <f t="shared" si="1"/>
@@ -2698,14 +2667,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B9" s="15">
         <v>0</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="1"/>
@@ -2714,14 +2683,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B10" s="15">
         <v>0</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="1"/>
@@ -2730,14 +2699,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="1"/>
@@ -2746,14 +2715,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B12" s="27">
         <v>1</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="49" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E12" s="12">
         <f t="shared" si="1"/>
@@ -2762,13 +2731,13 @@
     </row>
     <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>227</v>
-      </c>
-      <c r="B13" s="15">
-        <v>0</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>235</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="1"/>
@@ -2777,13 +2746,13 @@
     </row>
     <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>228</v>
-      </c>
-      <c r="B14" s="15">
-        <v>0</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>236</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="1"/>
@@ -2792,14 +2761,14 @@
     </row>
     <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="80" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B15" s="20">
         <v>0</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="17" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E15" s="14">
         <f t="shared" si="1"/>
@@ -2817,7 +2786,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E16" s="14">
         <f t="shared" si="1"/>
@@ -2832,10 +2801,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="1"/>
@@ -2850,10 +2819,10 @@
         <v>0</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="1"/>
@@ -2868,10 +2837,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E19" s="70">
         <f t="shared" si="1"/>
@@ -2879,21 +2848,21 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B20" s="75">
-        <v>1737</v>
-      </c>
-      <c r="C20" s="29" t="s">
+      <c r="B20" s="74">
+        <v>0</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="E20" s="65">
+      <c r="D20" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="70">
         <f t="shared" si="1"/>
-        <v>1737000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2903,11 +2872,11 @@
       <c r="B21" s="75">
         <v>0</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>52</v>
+      <c r="C21" s="72" t="s">
+        <v>193</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E21" s="65">
         <f t="shared" si="1"/>
@@ -2915,19 +2884,19 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+      <c r="A22" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="74">
-        <v>0</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E22" s="70">
+      <c r="B22" s="75">
+        <v>0</v>
+      </c>
+      <c r="C22" s="72" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2939,85 +2908,13 @@
       <c r="B23" s="74">
         <v>0</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>238</v>
+      <c r="C23" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>196</v>
       </c>
       <c r="E23" s="70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>189</v>
-      </c>
-      <c r="B24" s="75">
-        <v>0</v>
-      </c>
-      <c r="C24" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E24" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>190</v>
-      </c>
-      <c r="B25" s="75">
-        <v>0</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="D25" t="s">
-        <v>201</v>
-      </c>
-      <c r="E25" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B26" s="74">
-        <v>0</v>
-      </c>
-      <c r="C26" s="77" t="s">
-        <v>199</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E26" s="70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="B27" s="9">
-        <v>0</v>
-      </c>
-      <c r="C27" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="E27" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3030,10 +2927,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C720B3-BEEA-4D2E-BE7C-7EC9578AFA75}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3096,7 +2993,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3108,12 +3005,12 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -3122,15 +3019,15 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -3139,10 +3036,10 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3156,24 +3053,24 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B8">
         <v>19</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>19</v>
@@ -3181,10 +3078,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>22</v>
@@ -3193,60 +3090,43 @@
         <v>20</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>38</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <f>B2</f>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>21</v>
+        <f>D2</f>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11">
-        <f>B2</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <f>D2</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>25</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3258,8 +3138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD82E9-FB96-4FE4-9B12-1EDF4DE7082A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3322,7 +3202,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3356,7 +3236,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -3373,7 +3253,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3436,7 +3316,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3704,13 +3584,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B15" s="9">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
@@ -3719,7 +3599,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B16" s="26">
         <f>0.00000016*3</f>
@@ -3731,7 +3611,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B17" s="9">
         <v>0</v>
@@ -3739,7 +3619,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B18" s="9">
         <v>0</v>
@@ -3747,7 +3627,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -5059,7 +4939,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B8" s="76">
         <v>1</v>
@@ -5068,7 +4948,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="76" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E8" s="79">
         <f>B8/1000</f>
@@ -5078,16 +4958,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B9" s="6">
         <v>2</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E9" s="42">
         <f>B9/1000</f>
@@ -5097,16 +4977,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B10" s="6">
         <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E10" s="42">
         <f>B10/1000</f>
@@ -5116,16 +4996,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B11" s="8">
         <v>180</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E11" s="43">
         <f t="shared" ref="E11:E15" si="1">RADIANS(B11)/3600</f>
@@ -5135,7 +5015,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="78" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B12" s="76">
         <v>150</v>
@@ -5144,7 +5024,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="76" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E12" s="79">
         <f t="shared" si="1"/>
@@ -5154,16 +5034,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B13" s="6">
         <v>0.01</v>
       </c>
       <c r="C13" s="72" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E13" s="42">
         <f t="shared" si="1"/>
@@ -5173,16 +5053,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B14" s="6">
         <v>0.02</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E14" s="42">
         <f t="shared" si="1"/>
@@ -5192,16 +5072,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B15" s="8">
         <v>0.03</v>
       </c>
       <c r="C15" s="77" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Debugging, adding additional plots
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E571A1B-016B-8C4D-8E0B-3BD376D7F2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1962DC-1E06-8545-A300-E265D8DC7191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="263">
   <si>
     <t>Value</t>
   </si>
@@ -1446,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1518,8 +1518,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="64">
-        <f>B5*0.5</f>
-        <v>3404.7101009954345</v>
+        <v>550</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>5</v>
@@ -1529,7 +1528,7 @@
       </c>
       <c r="E4" s="65">
         <f t="shared" si="0"/>
-        <v>3404.7101009954345</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2279,7 +2278,7 @@
         <v>247</v>
       </c>
       <c r="B46" s="2">
-        <v>1.6242000000000001</v>
+        <v>0</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>193</v>
@@ -2289,7 +2288,7 @@
       </c>
       <c r="E46" s="1">
         <f t="shared" ref="E46" si="9">B46</f>
-        <v>1.6242000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2369,7 +2368,7 @@
         <v>249</v>
       </c>
       <c r="B51" s="2">
-        <v>-1738</v>
+        <v>1738</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>52</v>
@@ -2378,8 +2377,8 @@
         <v>246</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" ref="E51:E54" si="11">B51</f>
-        <v>-1738</v>
+        <f>B51*1000</f>
+        <v>1738000</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2396,7 +2395,7 @@
         <v>246</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="E51:E54" si="11">B52</f>
         <v>0</v>
       </c>
     </row>
@@ -2511,7 +2510,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2554,7 +2553,7 @@
         <v>72</v>
       </c>
       <c r="E2" s="31">
-        <f t="shared" ref="E2:E4" si="0">B2*1000</f>
+        <f>B2*1000</f>
         <v>-390000</v>
       </c>
       <c r="G2" s="9"/>
@@ -2563,8 +2562,9 @@
       <c r="A3" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="33">
-        <v>10.3957</v>
+      <c r="B3" s="9">
+        <f>10.3957+1737.5</f>
+        <v>1747.8957</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>52</v>
@@ -2573,8 +2573,8 @@
         <v>74</v>
       </c>
       <c r="E3" s="31">
-        <f t="shared" si="0"/>
-        <v>10395.699999999999</v>
+        <f t="shared" ref="E2:E4" si="0">B3*1000</f>
+        <v>1747895.7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="33">
-        <v>-0.58329957806655397</v>
+        <v>0</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>78</v>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="E7" s="31">
         <f t="shared" si="1"/>
-        <v>-583.29957806655398</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2654,7 +2654,7 @@
         <v>214</v>
       </c>
       <c r="B8" s="27">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="E8" s="12">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2718,15 +2718,17 @@
         <v>218</v>
       </c>
       <c r="B12" s="27">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="D12" s="49" t="s">
         <v>226</v>
       </c>
       <c r="E12" s="12">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+        <f>B12*1000</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3138,7 +3140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD82E9-FB96-4FE4-9B12-1EDF4DE7082A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -3316,7 +3318,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4789,7 +4791,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4942,7 +4944,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="76">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C8" s="76" t="s">
         <v>8</v>
@@ -4952,7 +4954,7 @@
       </c>
       <c r="E8" s="79">
         <f>B8/1000</f>
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F8" s="6"/>
     </row>
@@ -4961,7 +4963,7 @@
         <v>202</v>
       </c>
       <c r="B9" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>213</v>
@@ -4971,7 +4973,7 @@
       </c>
       <c r="E9" s="42">
         <f>B9/1000</f>
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -4980,7 +4982,7 @@
         <v>203</v>
       </c>
       <c r="B10" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>213</v>
@@ -4990,7 +4992,7 @@
       </c>
       <c r="E10" s="42">
         <f>B10/1000</f>
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="F10" s="6"/>
     </row>
@@ -4999,7 +5001,7 @@
         <v>204</v>
       </c>
       <c r="B11" s="8">
-        <v>180</v>
+        <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>213</v>
@@ -5009,7 +5011,7 @@
       </c>
       <c r="E11" s="43">
         <f t="shared" ref="E11:E15" si="1">RADIANS(B11)/3600</f>
-        <v>8.726646259971648E-4</v>
+        <v>1.454441043328608E-5</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -5018,7 +5020,7 @@
         <v>205</v>
       </c>
       <c r="B12" s="76">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C12" s="76" t="s">
         <v>8</v>
@@ -5028,7 +5030,7 @@
       </c>
       <c r="E12" s="79">
         <f t="shared" si="1"/>
-        <v>7.2722052166430398E-4</v>
+        <v>4.8481368110953597E-5</v>
       </c>
       <c r="F12" s="6"/>
     </row>
@@ -5037,7 +5039,7 @@
         <v>206</v>
       </c>
       <c r="B13" s="6">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C13" s="72" t="s">
         <v>193</v>
@@ -5047,7 +5049,7 @@
       </c>
       <c r="E13" s="42">
         <f t="shared" si="1"/>
-        <v>4.8481368110953601E-8</v>
+        <v>4.8481368110953598E-6</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -5056,7 +5058,7 @@
         <v>207</v>
       </c>
       <c r="B14" s="6">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>193</v>
@@ -5066,7 +5068,7 @@
       </c>
       <c r="E14" s="42">
         <f t="shared" si="1"/>
-        <v>9.6962736221907202E-8</v>
+        <v>4.8481368110953598E-6</v>
       </c>
       <c r="F14" s="6"/>
     </row>
@@ -5075,7 +5077,7 @@
         <v>208</v>
       </c>
       <c r="B15" s="8">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="C15" s="77" t="s">
         <v>193</v>
@@ -5085,7 +5087,7 @@
       </c>
       <c r="E15" s="43">
         <f t="shared" si="1"/>
-        <v>1.4544410433286078E-7</v>
+        <v>4.8481368110953598E-6</v>
       </c>
       <c r="F15" s="6"/>
     </row>

</xml_diff>

<commit_message>
Fixed a sign error!
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\epitts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4539DA88-DE71-4D4C-A18B-7677235756DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C2C60-BC1B-4469-A8AC-3F9513A445D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="465" windowWidth="16800" windowHeight="18915" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -29,24 +29,15 @@
     <definedName name="g2mps2">Constants!$B$4</definedName>
     <definedName name="hr2min">Constants!$B$1</definedName>
     <definedName name="hr2sec">Constants!$B$3</definedName>
+    <definedName name="km2m">Constants!$B$6</definedName>
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="259">
   <si>
     <t>Value</t>
   </si>
@@ -820,6 +811,9 @@
   </si>
   <si>
     <t>Moon gravitational constant</t>
+  </si>
+  <si>
+    <t>km2m</t>
   </si>
 </sst>
 </file>
@@ -1431,21 +1425,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1456,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
@@ -1480,7 +1474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1492,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
@@ -1516,7 +1510,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
@@ -1535,7 +1529,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
@@ -1571,7 +1565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>128</v>
       </c>
@@ -1590,7 +1584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
@@ -1608,7 +1602,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
@@ -1626,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
@@ -1644,7 +1638,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>45</v>
       </c>
@@ -1662,7 +1656,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1680,7 +1674,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1698,7 +1692,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>122</v>
       </c>
@@ -1716,7 +1710,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>48</v>
       </c>
@@ -1734,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
@@ -1752,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>50</v>
       </c>
@@ -1770,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>231</v>
       </c>
@@ -1789,7 +1783,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>251</v>
       </c>
@@ -1808,12 +1802,12 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>4</v>
@@ -1823,10 +1817,10 @@
       </c>
       <c r="E21" s="65">
         <f t="shared" ref="E21:E23" si="2">B21</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>20</v>
       </c>
@@ -1844,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>36</v>
       </c>
@@ -1862,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>144</v>
       </c>
@@ -1880,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>143</v>
       </c>
@@ -1898,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>142</v>
       </c>
@@ -1916,7 +1910,7 @@
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>148</v>
       </c>
@@ -1934,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>149</v>
       </c>
@@ -1952,7 +1946,7 @@
         <v>-1.5707963267948966</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>150</v>
       </c>
@@ -1970,7 +1964,7 @@
         <v>0.52359877559829882</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>139</v>
       </c>
@@ -1988,7 +1982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>141</v>
       </c>
@@ -2006,7 +2000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>161</v>
       </c>
@@ -2024,7 +2018,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>172</v>
       </c>
@@ -2042,7 +2036,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>164</v>
       </c>
@@ -2060,7 +2054,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>165</v>
       </c>
@@ -2078,7 +2072,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>173</v>
       </c>
@@ -2096,7 +2090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="50" t="s">
         <v>124</v>
       </c>
@@ -2114,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
         <v>125</v>
       </c>
@@ -2132,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
         <v>176</v>
       </c>
@@ -2150,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>177</v>
       </c>
@@ -2168,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>179</v>
       </c>
@@ -2186,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>233</v>
       </c>
@@ -2204,7 +2198,7 @@
         <v>1737.5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>234</v>
       </c>
@@ -2222,7 +2216,7 @@
         <v>1737.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>236</v>
       </c>
@@ -2240,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>238</v>
       </c>
@@ -2258,7 +2252,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>247</v>
       </c>
@@ -2276,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>240</v>
       </c>
@@ -2294,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>242</v>
       </c>
@@ -2312,7 +2306,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>248</v>
       </c>
@@ -2330,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>245</v>
       </c>
@@ -2348,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>249</v>
       </c>
@@ -2366,7 +2360,7 @@
         <v>1738000</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>250</v>
       </c>
@@ -2384,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>252</v>
       </c>
@@ -2402,7 +2396,7 @@
         <v>2.7E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>253</v>
       </c>
@@ -2420,7 +2414,7 @@
         <v>4904869500000</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
@@ -2433,18 +2427,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2452,7 +2446,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2460,7 +2454,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2469,7 +2463,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2477,12 +2471,20 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>160</v>
       </c>
       <c r="B5">
         <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -2495,19 +2497,19 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2524,7 +2526,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>71</v>
       </c>
@@ -2538,12 +2540,12 @@
         <v>72</v>
       </c>
       <c r="E2" s="31">
-        <f>B2*1000</f>
+        <f>B2*km2m</f>
         <v>-390000</v>
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>73</v>
       </c>
@@ -2558,11 +2560,11 @@
         <v>74</v>
       </c>
       <c r="E3" s="31">
-        <f t="shared" ref="E3:E4" si="0">B3*1000</f>
+        <f>B3*km2m</f>
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>75</v>
       </c>
@@ -2576,11 +2578,11 @@
         <v>76</v>
       </c>
       <c r="E4" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <f>B4*km2m</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>77</v>
       </c>
@@ -2594,11 +2596,11 @@
         <v>72</v>
       </c>
       <c r="E5" s="31">
-        <f t="shared" ref="E5:E23" si="1">B5*1000</f>
+        <f t="shared" ref="E5:E23" si="0">B5*1000</f>
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>79</v>
       </c>
@@ -2612,11 +2614,11 @@
         <v>74</v>
       </c>
       <c r="E6" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>80</v>
       </c>
@@ -2630,27 +2632,27 @@
         <v>76</v>
       </c>
       <c r="E7" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="81" t="s">
         <v>214</v>
       </c>
       <c r="B8" s="27">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
         <v>222</v>
       </c>
       <c r="E8" s="12">
-        <f t="shared" si="1"/>
+        <f>B8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>215</v>
       </c>
@@ -2662,11 +2664,11 @@
         <v>223</v>
       </c>
       <c r="E9" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <f>B9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>216</v>
       </c>
@@ -2678,11 +2680,11 @@
         <v>224</v>
       </c>
       <c r="E10" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <f>B10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
         <v>217</v>
       </c>
@@ -2694,27 +2696,27 @@
         <v>225</v>
       </c>
       <c r="E11" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <f>B11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>218</v>
       </c>
       <c r="B12" s="27">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="49" t="s">
         <v>226</v>
       </c>
       <c r="E12" s="12">
-        <f>B12*1000</f>
+        <f>B12</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>219</v>
       </c>
@@ -2725,11 +2727,11 @@
         <v>227</v>
       </c>
       <c r="E13" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <f>B13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>220</v>
       </c>
@@ -2740,11 +2742,11 @@
         <v>228</v>
       </c>
       <c r="E14" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <f>B14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="80" t="s">
         <v>221</v>
       </c>
@@ -2756,11 +2758,11 @@
         <v>229</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <f>B15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
         <v>181</v>
       </c>
@@ -2774,11 +2776,11 @@
         <v>192</v>
       </c>
       <c r="E16" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>182</v>
       </c>
@@ -2792,11 +2794,11 @@
         <v>189</v>
       </c>
       <c r="E17" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
         <v>183</v>
       </c>
@@ -2810,11 +2812,11 @@
         <v>190</v>
       </c>
       <c r="E18" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>184</v>
       </c>
@@ -2828,11 +2830,11 @@
         <v>191</v>
       </c>
       <c r="E19" s="70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>185</v>
       </c>
@@ -2846,11 +2848,11 @@
         <v>230</v>
       </c>
       <c r="E20" s="70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>186</v>
       </c>
@@ -2864,11 +2866,11 @@
         <v>194</v>
       </c>
       <c r="E21" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>187</v>
       </c>
@@ -2882,11 +2884,11 @@
         <v>195</v>
       </c>
       <c r="E22" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>188</v>
       </c>
@@ -2900,7 +2902,7 @@
         <v>196</v>
       </c>
       <c r="E23" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2918,14 +2920,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2959,7 +2961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2976,7 +2978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -2993,7 +2995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -3010,7 +3012,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>199</v>
       </c>
@@ -3027,7 +3029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -3044,7 +3046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -3061,7 +3063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -3078,7 +3080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3097,7 +3099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -3127,14 +3129,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3168,7 +3170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3185,7 +3187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3202,7 +3204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -3219,7 +3221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -3236,7 +3238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -3253,7 +3255,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3272,7 +3274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3304,17 +3306,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -3331,7 +3333,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>129</v>
       </c>
@@ -3350,7 +3352,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -3369,7 +3371,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3387,7 +3389,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>102</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>103</v>
       </c>
@@ -3423,7 +3425,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>104</v>
       </c>
@@ -3441,7 +3443,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>105</v>
       </c>
@@ -3459,7 +3461,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>106</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
@@ -3495,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>136</v>
       </c>
@@ -3513,7 +3515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>154</v>
       </c>
@@ -3531,7 +3533,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>156</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>158</v>
       </c>
@@ -3567,22 +3569,22 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="C15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="26"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
     </row>
   </sheetData>
@@ -3599,17 +3601,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3626,7 +3628,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
@@ -3644,7 +3646,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>88</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>89</v>
       </c>
@@ -3680,7 +3682,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>90</v>
       </c>
@@ -3698,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>93</v>
       </c>
@@ -3716,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>94</v>
       </c>
@@ -3734,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
@@ -3752,7 +3754,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>108</v>
       </c>
@@ -3770,7 +3772,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>109</v>
       </c>
@@ -3788,7 +3790,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>113</v>
       </c>
@@ -3807,7 +3809,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>114</v>
       </c>
@@ -3826,7 +3828,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>115</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>110</v>
       </c>
@@ -3864,7 +3866,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>111</v>
       </c>
@@ -3883,7 +3885,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>112</v>
       </c>
@@ -3902,7 +3904,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>98</v>
       </c>
@@ -3921,7 +3923,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -3940,7 +3942,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>101</v>
       </c>
@@ -3971,18 +3973,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -3999,7 +4001,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -4022,7 +4024,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -4045,7 +4047,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -4068,7 +4070,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -4091,7 +4093,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -4113,7 +4115,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -4135,7 +4137,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -4157,7 +4159,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -4179,7 +4181,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -4201,7 +4203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -4223,7 +4225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -4245,7 +4247,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -4267,7 +4269,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -4303,17 +4305,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4330,7 +4332,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -4353,7 +4355,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -4376,7 +4378,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -4399,7 +4401,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -4422,7 +4424,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -4444,7 +4446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -4466,7 +4468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4488,7 +4490,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4510,7 +4512,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4532,7 +4534,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4554,7 +4556,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4576,7 +4578,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4598,7 +4600,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4620,7 +4622,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4642,7 +4644,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4664,7 +4666,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4686,7 +4688,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4708,7 +4710,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4744,15 +4746,15 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4769,7 +4771,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>116</v>
       </c>
@@ -4789,7 +4791,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>117</v>
       </c>
@@ -4809,7 +4811,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>118</v>
       </c>
@@ -4829,7 +4831,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>119</v>
       </c>
@@ -4849,7 +4851,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -4869,7 +4871,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>121</v>
       </c>
@@ -4889,7 +4891,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
         <v>201</v>
       </c>
@@ -4908,7 +4910,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>202</v>
       </c>
@@ -4927,7 +4929,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>203</v>
       </c>
@@ -4946,7 +4948,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>204</v>
       </c>
@@ -4965,7 +4967,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
         <v>205</v>
       </c>
@@ -4984,7 +4986,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>206</v>
       </c>
@@ -5003,7 +5005,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>207</v>
       </c>
@@ -5022,7 +5024,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>208</v>
       </c>
@@ -5041,7 +5043,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5049,7 +5051,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5057,7 +5059,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5065,7 +5067,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5073,7 +5075,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>

</xml_diff>

<commit_message>
Working on linear error state modeling
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\epitts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C2C60-BC1B-4469-A8AC-3F9513A445D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEC735-B9F8-0B4C-A731-732BCD7AE359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="465" windowWidth="16800" windowHeight="18915" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -33,11 +33,21 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="260">
   <si>
     <t>Value</t>
   </si>
@@ -814,6 +824,9 @@
   </si>
   <si>
     <t>km2m</t>
+  </si>
+  <si>
+    <t>errorPropTestEnable1</t>
   </si>
 </sst>
 </file>
@@ -1423,23 +1436,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
@@ -1456,7 +1469,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
@@ -1474,7 +1487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1492,7 +1505,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
@@ -1529,7 +1542,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1547,7 +1560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
@@ -1565,7 +1578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>128</v>
       </c>
@@ -1584,7 +1597,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
@@ -1602,7 +1615,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
@@ -1620,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
@@ -1638,7 +1651,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>45</v>
       </c>
@@ -1656,7 +1669,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +1687,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
@@ -1692,7 +1705,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>122</v>
       </c>
@@ -1710,7 +1723,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>48</v>
       </c>
@@ -1728,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
@@ -1746,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>50</v>
       </c>
@@ -1764,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>231</v>
       </c>
@@ -1783,7 +1796,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>251</v>
       </c>
@@ -1802,7 +1815,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>34</v>
       </c>
@@ -1816,31 +1829,27 @@
         <v>35</v>
       </c>
       <c r="E21" s="65">
-        <f t="shared" ref="E21:E23" si="2">B21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E21:E24" si="2">B21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" s="66">
+        <v>1</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="65">
+        <f>B22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" s="66">
-        <v>0</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="65">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>36</v>
       </c>
       <c r="B23" s="66">
         <v>0</v>
@@ -1849,34 +1858,34 @@
         <v>4</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E23" s="65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="66">
+        <v>0</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="65">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
         <v>144</v>
-      </c>
-      <c r="B24" s="64">
-        <v>0</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E24" s="65">
-        <f t="shared" ref="E24:E29" si="3">RADIANS(B24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="B25" s="64">
         <v>0</v>
@@ -1885,178 +1894,178 @@
         <v>22</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E25" s="65">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E25:E30" si="3">RADIANS(B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B26" s="64">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" s="65">
         <f t="shared" si="3"/>
-        <v>3.1415926535897931</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B27" s="64">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E27" s="65">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.1415926535897931</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B28" s="64">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E28" s="65">
         <f t="shared" si="3"/>
-        <v>-1.5707963267948966</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B29" s="64">
-        <v>30</v>
+        <v>-90</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E29" s="65">
         <f t="shared" si="3"/>
-        <v>0.52359877559829882</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B30" s="64">
         <v>30</v>
       </c>
       <c r="C30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="65">
+        <f t="shared" si="3"/>
+        <v>0.52359877559829882</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="64">
+        <v>30</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D31" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="E30" s="65">
-        <f t="shared" ref="E30:E31" si="4">B30</f>
+      <c r="E31" s="65">
+        <f t="shared" ref="E31:E32" si="4">B31</f>
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="64">
-        <v>0</v>
-      </c>
-      <c r="C31" s="16" t="s">
+      <c r="B32" s="64">
+        <v>0</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D32" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E32" s="65">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="B32" s="64">
+      <c r="B33" s="64">
         <v>19</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C33" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D33" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="E32" s="65">
-        <f>B32/1000</f>
+      <c r="E33" s="65">
+        <f>B33/1000</f>
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="64">
+      <c r="B34" s="64">
         <v>7</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C34" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="65">
-        <f>B33*0.000001</f>
+      <c r="E34" s="65">
+        <f>B34*0.000001</f>
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
         <v>164</v>
-      </c>
-      <c r="B34" s="64">
-        <v>2500</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" s="65">
-        <f t="shared" ref="E34:E35" si="5">B34</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>165</v>
       </c>
       <c r="B35" s="64">
         <v>2500</v>
@@ -2065,142 +2074,142 @@
         <v>134</v>
       </c>
       <c r="D35" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="65">
+        <f t="shared" ref="E35:E36" si="5">B35</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="64">
+        <v>2500</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E36" s="65">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="66">
+      <c r="B37" s="66">
         <v>5</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C37" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D37" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="E36" s="65">
-        <f>B36</f>
+      <c r="E37" s="65">
+        <f>B37</f>
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="B37" s="51">
+      <c r="B38" s="51">
         <v>1</v>
       </c>
-      <c r="C37" s="52" t="s">
+      <c r="C38" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="52" t="s">
+      <c r="D38" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E37" s="53">
-        <f t="shared" ref="E37:E39" si="6">B37</f>
+      <c r="E38" s="53">
+        <f t="shared" ref="E38:E40" si="6">B38</f>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="55">
+      <c r="B39" s="55">
         <v>1</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C39" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D39" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="E38" s="57">
+      <c r="E39" s="57">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="48" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="B39" s="71">
-        <v>0</v>
-      </c>
-      <c r="C39" s="49" t="s">
+      <c r="B40" s="71">
+        <v>0</v>
+      </c>
+      <c r="C40" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="49" t="s">
+      <c r="D40" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="E39" s="63">
+      <c r="E40" s="63">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="B40" s="66">
-        <v>0</v>
-      </c>
-      <c r="C40" s="16" t="s">
+      <c r="B41" s="66">
+        <v>0</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D41" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="E40" s="65">
-        <f t="shared" ref="E40" si="7">B40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="E41" s="65">
+        <f t="shared" ref="E41" si="7">B41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="69">
-        <v>0</v>
-      </c>
-      <c r="C41" s="17" t="s">
+      <c r="B42" s="69">
+        <v>0</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D42" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="70">
-        <f t="shared" ref="E41:E50" si="8">B41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="E42" s="70">
+        <f t="shared" ref="E42:E51" si="8">B42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
         <v>233</v>
-      </c>
-      <c r="B42" s="2">
-        <v>1737.5</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" si="8"/>
-        <v>1737.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>234</v>
       </c>
       <c r="B43" s="2">
         <v>1737.5</v>
@@ -2216,48 +2225,48 @@
         <v>1737.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B44" s="2">
-        <v>0</v>
+        <v>1737.5</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>193</v>
+        <v>52</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1737.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B45" s="2">
-        <v>1.62</v>
+        <v>0</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>193</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" s="2">
         <v>1.62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B46" s="2">
-        <v>0</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>193</v>
@@ -2266,52 +2275,52 @@
         <v>239</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" ref="E46" si="9">B46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" ref="E47" si="9">B47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="B47" s="2">
-        <v>0</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="E47" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
-        <v>242</v>
-      </c>
       <c r="B48" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>243</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="B49" s="2">
         <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>243</v>
@@ -2320,34 +2329,34 @@
         <v>244</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" ref="E49" si="10">B49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" ref="E50" si="10">B50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B50" s="2">
-        <v>0</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="E50" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>249</v>
-      </c>
       <c r="B51" s="2">
-        <v>1738</v>
+        <v>0</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>52</v>
@@ -2356,16 +2365,16 @@
         <v>246</v>
       </c>
       <c r="E51" s="1">
-        <f>B51*1000</f>
-        <v>1738000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B52" s="2">
-        <v>0</v>
+        <v>1738</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>52</v>
@@ -2374,50 +2383,68 @@
         <v>246</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:E54" si="11">B52</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <f>B52*1000</f>
+        <v>1738000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" ref="E53:E55" si="11">B53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="B53" s="82">
+      <c r="B54" s="82">
         <v>2.7E-6</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>254</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>255</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E54" s="1">
         <f t="shared" si="11"/>
         <v>2.7E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="B54" s="83">
+      <c r="B55" s="83">
         <v>4904869500000</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>256</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>257</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E55" s="1">
         <f t="shared" si="11"/>
         <v>4904869500000</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="18"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2433,12 +2460,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2446,7 +2473,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2454,7 +2481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2463,7 +2490,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2471,7 +2498,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -2479,7 +2506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>258</v>
       </c>
@@ -2500,16 +2527,16 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2526,7 +2553,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>71</v>
       </c>
@@ -2545,7 +2572,7 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>73</v>
       </c>
@@ -2564,7 +2591,7 @@
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>75</v>
       </c>
@@ -2582,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>77</v>
       </c>
@@ -2600,7 +2627,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>79</v>
       </c>
@@ -2618,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>80</v>
       </c>
@@ -2636,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
         <v>214</v>
       </c>
@@ -2648,11 +2675,11 @@
         <v>222</v>
       </c>
       <c r="E8" s="12">
-        <f>B8</f>
+        <f t="shared" ref="E8:E15" si="1">B8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>215</v>
       </c>
@@ -2664,11 +2691,11 @@
         <v>223</v>
       </c>
       <c r="E9" s="13">
-        <f>B9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>216</v>
       </c>
@@ -2680,11 +2707,11 @@
         <v>224</v>
       </c>
       <c r="E10" s="13">
-        <f>B10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
         <v>217</v>
       </c>
@@ -2696,11 +2723,11 @@
         <v>225</v>
       </c>
       <c r="E11" s="13">
-        <f>B11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>218</v>
       </c>
@@ -2712,11 +2739,11 @@
         <v>226</v>
       </c>
       <c r="E12" s="12">
-        <f>B12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>219</v>
       </c>
@@ -2727,11 +2754,11 @@
         <v>227</v>
       </c>
       <c r="E13" s="13">
-        <f>B13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>220</v>
       </c>
@@ -2742,11 +2769,11 @@
         <v>228</v>
       </c>
       <c r="E14" s="13">
-        <f>B14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="80" t="s">
         <v>221</v>
       </c>
@@ -2758,11 +2785,11 @@
         <v>229</v>
       </c>
       <c r="E15" s="14">
-        <f>B15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="47" t="s">
         <v>181</v>
       </c>
@@ -2780,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
         <v>182</v>
       </c>
@@ -2798,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>183</v>
       </c>
@@ -2816,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>184</v>
       </c>
@@ -2834,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>185</v>
       </c>
@@ -2852,7 +2879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>186</v>
       </c>
@@ -2870,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>187</v>
       </c>
@@ -2888,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>188</v>
       </c>
@@ -2920,14 +2947,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2944,7 +2971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2961,7 +2988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2978,7 +3005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -2995,7 +3022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -3012,7 +3039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>199</v>
       </c>
@@ -3029,7 +3056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -3046,7 +3073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -3063,7 +3090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -3080,7 +3107,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3099,7 +3126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -3129,14 +3156,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3153,7 +3180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3170,7 +3197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3187,7 +3214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3204,7 +3231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -3221,7 +3248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -3238,7 +3265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -3255,7 +3282,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3274,7 +3301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3306,17 +3333,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -3333,7 +3360,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>129</v>
       </c>
@@ -3352,7 +3379,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -3371,7 +3398,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3389,7 +3416,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>102</v>
       </c>
@@ -3407,7 +3434,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>103</v>
       </c>
@@ -3425,7 +3452,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>104</v>
       </c>
@@ -3443,7 +3470,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>105</v>
       </c>
@@ -3461,7 +3488,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>106</v>
       </c>
@@ -3479,7 +3506,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
@@ -3497,7 +3524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>136</v>
       </c>
@@ -3515,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>154</v>
       </c>
@@ -3533,7 +3560,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>156</v>
       </c>
@@ -3551,7 +3578,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>158</v>
       </c>
@@ -3569,22 +3596,22 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="C15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="26"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
     </row>
   </sheetData>
@@ -3601,17 +3628,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3628,7 +3655,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
@@ -3646,7 +3673,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>88</v>
       </c>
@@ -3664,7 +3691,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>89</v>
       </c>
@@ -3682,7 +3709,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>90</v>
       </c>
@@ -3700,7 +3727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>93</v>
       </c>
@@ -3718,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>94</v>
       </c>
@@ -3736,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
@@ -3754,7 +3781,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>108</v>
       </c>
@@ -3772,7 +3799,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>109</v>
       </c>
@@ -3790,7 +3817,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>113</v>
       </c>
@@ -3809,7 +3836,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>114</v>
       </c>
@@ -3828,7 +3855,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>115</v>
       </c>
@@ -3847,7 +3874,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>110</v>
       </c>
@@ -3866,7 +3893,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>111</v>
       </c>
@@ -3885,7 +3912,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>112</v>
       </c>
@@ -3904,7 +3931,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>98</v>
       </c>
@@ -3923,7 +3950,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -3942,7 +3969,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>101</v>
       </c>
@@ -3973,18 +4000,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4001,7 +4028,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -4024,7 +4051,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -4047,7 +4074,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -4070,7 +4097,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -4093,7 +4120,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -4115,7 +4142,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -4137,7 +4164,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -4159,7 +4186,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -4181,7 +4208,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -4203,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -4225,7 +4252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -4247,7 +4274,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -4269,7 +4296,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -4305,17 +4332,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4332,7 +4359,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -4355,7 +4382,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -4378,7 +4405,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -4401,7 +4428,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -4424,7 +4451,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -4446,7 +4473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -4468,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4490,7 +4517,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4512,7 +4539,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4534,7 +4561,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4556,7 +4583,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4578,7 +4605,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4600,7 +4627,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4622,7 +4649,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4644,7 +4671,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4666,7 +4693,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4688,7 +4715,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4710,7 +4737,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4746,15 +4773,15 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -4771,7 +4798,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>116</v>
       </c>
@@ -4791,7 +4818,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>117</v>
       </c>
@@ -4811,7 +4838,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>118</v>
       </c>
@@ -4831,7 +4858,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>119</v>
       </c>
@@ -4851,7 +4878,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -4871,7 +4898,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>121</v>
       </c>
@@ -4891,7 +4918,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
         <v>201</v>
       </c>
@@ -4910,7 +4937,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>202</v>
       </c>
@@ -4929,7 +4956,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>203</v>
       </c>
@@ -4948,7 +4975,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>204</v>
       </c>
@@ -4967,7 +4994,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="78" t="s">
         <v>205</v>
       </c>
@@ -4986,7 +5013,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>206</v>
       </c>
@@ -5005,7 +5032,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>207</v>
       </c>
@@ -5024,7 +5051,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>208</v>
       </c>
@@ -5043,7 +5070,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5051,7 +5078,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5059,7 +5086,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5067,7 +5094,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5075,7 +5102,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>

</xml_diff>

<commit_message>
Finishing the non-linear error modeling and cleaning up files
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEC735-B9F8-0B4C-A731-732BCD7AE359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A75E1D7-579C-CC4F-BC53-B40ADBD05393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <definedName name="g2mps2">Constants!$B$4</definedName>
     <definedName name="hr2min">Constants!$B$1</definedName>
     <definedName name="hr2sec">Constants!$B$3</definedName>
-    <definedName name="km2m">Constants!$B$6</definedName>
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="256">
   <si>
     <t>Value</t>
   </si>
@@ -475,121 +474,259 @@
     <t>alpha</t>
   </si>
   <si>
+    <t>thz_c</t>
+  </si>
+  <si>
+    <t>thy_c</t>
+  </si>
+  <si>
+    <t>thx_c</t>
+  </si>
+  <si>
+    <t>z angle of a ZYX euler angle sequence to define C orientation wrt body</t>
+  </si>
+  <si>
+    <t>y angle of a ZYX euler angle sequence to define C orientation wrt body</t>
+  </si>
+  <si>
+    <t>x angle of a ZYX euler angle sequence to define C orientation wrt body</t>
+  </si>
+  <si>
+    <t>sig_idpos</t>
+  </si>
+  <si>
+    <t>3-sigma change in inertial position measurement uncertainty</t>
+  </si>
+  <si>
+    <t>sig_loss</t>
+  </si>
+  <si>
+    <t>3-sigma LOSS feature location uncertainty</t>
+  </si>
+  <si>
+    <t>sig_mdpos</t>
+  </si>
+  <si>
+    <t>3-sigma change in lunar-referenced position measurement uncertainty</t>
+  </si>
+  <si>
+    <t>days2hrs</t>
+  </si>
+  <si>
+    <t>focal_length</t>
+  </si>
+  <si>
+    <t>microns</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Hresolution</t>
+  </si>
+  <si>
+    <t>Vresolution</t>
+  </si>
+  <si>
+    <t>camera focal length</t>
+  </si>
+  <si>
+    <t>pixel pitch</t>
+  </si>
+  <si>
+    <t>horizontal resolution</t>
+  </si>
+  <si>
+    <t>vertical resolution</t>
+  </si>
+  <si>
+    <t>detector skewness</t>
+  </si>
+  <si>
+    <t>number of features to detect</t>
+  </si>
+  <si>
+    <t>pixel_pitch</t>
+  </si>
+  <si>
+    <t>vo_iterations</t>
+  </si>
+  <si>
+    <t>number of MLE iterations to refine the direction of motion estimate</t>
+  </si>
+  <si>
+    <t>flag to enable printing of VO diagnostic data</t>
+  </si>
+  <si>
+    <t>vo_diagnostics_enable</t>
+  </si>
+  <si>
+    <t>use_approx_cam_attitude_change_enable</t>
+  </si>
+  <si>
+    <t>flag to enable approximate modeling or moon-referenced camera attitude change</t>
+  </si>
+  <si>
+    <t>correlated_kalman_update_enable</t>
+  </si>
+  <si>
+    <t>flag to enable correlated Kalman update</t>
+  </si>
+  <si>
+    <t>Initial vechivle attitude quaternion</t>
+  </si>
+  <si>
+    <t>Injected range bias error</t>
+  </si>
+  <si>
+    <t>Injected gravity bias error</t>
+  </si>
+  <si>
+    <t>Injected terrain height error</t>
+  </si>
+  <si>
+    <t>Injected accelerometer bias error</t>
+  </si>
+  <si>
+    <t>Initial camera oreintation quaternion</t>
+  </si>
+  <si>
+    <t>Initial range bias</t>
+  </si>
+  <si>
+    <t>x component of intial gravity bias</t>
+  </si>
+  <si>
+    <t>y component of intial gravity bias</t>
+  </si>
+  <si>
+    <t>z component of intial gravity bias</t>
+  </si>
+  <si>
+    <t>Initial height of terrain</t>
+  </si>
+  <si>
+    <t>x component of initial accelerometer bias</t>
+  </si>
+  <si>
+    <t>y component of initial accelerometer bias</t>
+  </si>
+  <si>
+    <t>tau_r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range Bias time constant </t>
+  </si>
+  <si>
+    <t>d_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance correlation in gravity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_h </t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance correlation in height </t>
+  </si>
+  <si>
+    <t>m/s2</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Desired downrange accl at final time</t>
+  </si>
+  <si>
+    <t>Desired vertical accl at final time</t>
+  </si>
+  <si>
+    <t>Desired downrange vel at final time</t>
+  </si>
+  <si>
+    <t>desired toucdown velocity</t>
+  </si>
+  <si>
+    <t>Desired x postion at final time</t>
+  </si>
+  <si>
+    <t>Desired y postion at final time</t>
+  </si>
+  <si>
+    <t>Desired z postion at final time</t>
+  </si>
+  <si>
+    <t>omega_moon</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>rad/s</t>
+  </si>
+  <si>
+    <t>Moon rotation rate</t>
+  </si>
+  <si>
+    <t>m3/s2</t>
+  </si>
+  <si>
+    <t>Moon gravitational constant</t>
+  </si>
+  <si>
+    <t>tau_a</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>m/s3</t>
+  </si>
+  <si>
+    <t>m/s4</t>
+  </si>
+  <si>
+    <t>thz_st</t>
+  </si>
+  <si>
+    <t>z angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
+  </si>
+  <si>
+    <t>thy_st</t>
+  </si>
+  <si>
+    <t>y angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
+  </si>
+  <si>
     <t>thx_st</t>
   </si>
   <si>
-    <t>thy_st</t>
-  </si>
-  <si>
-    <t>thz_st</t>
-  </si>
-  <si>
-    <t>z angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
-    <t>y angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
     <t>x angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
   </si>
   <si>
-    <t>thz_c</t>
-  </si>
-  <si>
-    <t>thy_c</t>
-  </si>
-  <si>
-    <t>thx_c</t>
-  </si>
-  <si>
-    <t>z angle of a ZYX euler angle sequence to define C orientation wrt body</t>
-  </si>
-  <si>
-    <t>y angle of a ZYX euler angle sequence to define C orientation wrt body</t>
-  </si>
-  <si>
-    <t>x angle of a ZYX euler angle sequence to define C orientation wrt body</t>
-  </si>
-  <si>
-    <t>sig_idpos</t>
-  </si>
-  <si>
-    <t>3-sigma change in inertial position measurement uncertainty</t>
-  </si>
-  <si>
-    <t>sig_loss</t>
-  </si>
-  <si>
-    <t>3-sigma LOSS feature location uncertainty</t>
-  </si>
-  <si>
-    <t>sig_mdpos</t>
-  </si>
-  <si>
-    <t>3-sigma change in lunar-referenced position measurement uncertainty</t>
-  </si>
-  <si>
-    <t>days2hrs</t>
-  </si>
-  <si>
-    <t>focal_length</t>
-  </si>
-  <si>
-    <t>microns</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>Hresolution</t>
-  </si>
-  <si>
-    <t>Vresolution</t>
-  </si>
-  <si>
-    <t>camera focal length</t>
-  </si>
-  <si>
-    <t>pixel pitch</t>
-  </si>
-  <si>
-    <t>horizontal resolution</t>
-  </si>
-  <si>
-    <t>vertical resolution</t>
-  </si>
-  <si>
-    <t>detector skewness</t>
-  </si>
-  <si>
-    <t>number of features to detect</t>
-  </si>
-  <si>
-    <t>pixel_pitch</t>
-  </si>
-  <si>
-    <t>vo_iterations</t>
-  </si>
-  <si>
-    <t>number of MLE iterations to refine the direction of motion estimate</t>
-  </si>
-  <si>
-    <t>flag to enable printing of VO diagnostic data</t>
-  </si>
-  <si>
-    <t>vo_diagnostics_enable</t>
-  </si>
-  <si>
-    <t>use_approx_cam_attitude_change_enable</t>
-  </si>
-  <si>
-    <t>flag to enable approximate modeling or moon-referenced camera attitude change</t>
-  </si>
-  <si>
-    <t>correlated_kalman_update_enable</t>
-  </si>
-  <si>
-    <t>flag to enable correlated Kalman update</t>
+    <t>qm_i_a</t>
+  </si>
+  <si>
+    <t>qm_i_i</t>
+  </si>
+  <si>
+    <t>qm_i_j</t>
+  </si>
+  <si>
+    <t>qm_i_k</t>
+  </si>
+  <si>
+    <t>qc_b_a</t>
+  </si>
+  <si>
+    <t>qc_b_i</t>
+  </si>
+  <si>
+    <t>qc_b_j</t>
+  </si>
+  <si>
+    <t>qc_b_k</t>
   </si>
   <si>
     <t>b_r</t>
@@ -616,30 +753,6 @@
     <t>ba_z</t>
   </si>
   <si>
-    <t>x component of bias in gravity of the moon</t>
-  </si>
-  <si>
-    <t>y component of bias in gravity of the moon</t>
-  </si>
-  <si>
-    <t>z component of bias in gravity of the moon</t>
-  </si>
-  <si>
-    <t>clock bias, seen as bias in the measured range</t>
-  </si>
-  <si>
-    <t>m/s^2</t>
-  </si>
-  <si>
-    <t>x component of bias in the accelerometer in the body frame</t>
-  </si>
-  <si>
-    <t>y component of bias in the accelerometer in the body frame</t>
-  </si>
-  <si>
-    <t>z component of bias in the accelerometer in the body frame</t>
-  </si>
-  <si>
     <t>q_moon</t>
   </si>
   <si>
@@ -676,157 +789,31 @@
     <t>del_b_accel_z</t>
   </si>
   <si>
-    <t>Injected clock bias error</t>
-  </si>
-  <si>
-    <t>Injected gravitational bias error</t>
-  </si>
-  <si>
-    <t>injected feature height error</t>
-  </si>
-  <si>
-    <t>injected accelerometer error</t>
-  </si>
-  <si>
-    <t>m/sec^2</t>
-  </si>
-  <si>
-    <t>qm_i_a</t>
-  </si>
-  <si>
-    <t>qm_i_i</t>
-  </si>
-  <si>
-    <t>qm_i_j</t>
-  </si>
-  <si>
-    <t>qm_i_k</t>
-  </si>
-  <si>
-    <t>qc_b_a</t>
-  </si>
-  <si>
-    <t>qc_b_i</t>
-  </si>
-  <si>
-    <t>qc_b_j</t>
-  </si>
-  <si>
-    <t>qc_b_k</t>
-  </si>
-  <si>
-    <t>real component of the orientation in the inertial frame with respect to the moon</t>
-  </si>
-  <si>
-    <t>i component of the orientation in the inertial frame with respect to the moon</t>
-  </si>
-  <si>
-    <t>j component of the orientation in the inertial frame with respect to the moon</t>
-  </si>
-  <si>
-    <t>k component of the orientation in the inertial frame with respect to the moon</t>
-  </si>
-  <si>
-    <t>scalar component of the orientation of the body frame with respect to the camera</t>
-  </si>
-  <si>
-    <t>i component of the orientation of the body frame with respect to the camera</t>
-  </si>
-  <si>
-    <t>j component of the orientation of the body frame with respect to the camera</t>
-  </si>
-  <si>
-    <t>k component of the orientation of the body frame with respect to the camera</t>
-  </si>
-  <si>
-    <t>initial height of the terrain relative to the reference sphere</t>
-  </si>
-  <si>
-    <t>tau_r</t>
-  </si>
-  <si>
-    <t>Range bias ECRV time constant</t>
-  </si>
-  <si>
-    <t>d_g</t>
-  </si>
-  <si>
-    <t>d_h</t>
-  </si>
-  <si>
-    <t>Distance correlation for height</t>
-  </si>
-  <si>
     <t>astar_x_tf</t>
   </si>
   <si>
-    <t>Desired downrange acceleration at final time</t>
-  </si>
-  <si>
     <t>astar_y_tf</t>
   </si>
   <si>
-    <t>Desired vertical acceleration at final time</t>
+    <t>astar_z_tf</t>
   </si>
   <si>
     <t>vstar_x_tf</t>
   </si>
   <si>
-    <t>Desired downrange velocity at final time</t>
-  </si>
-  <si>
     <t>vstar_y_tf</t>
   </si>
   <si>
-    <t>m/s</t>
-  </si>
-  <si>
-    <t>Desired vertical velocity at final time</t>
+    <t>vstar_z_tf</t>
   </si>
   <si>
     <t>rstar_x_tf</t>
   </si>
   <si>
-    <t>Desired downrange position at final time</t>
-  </si>
-  <si>
-    <t>astar_z_tf</t>
-  </si>
-  <si>
-    <t>vstar_z_tf</t>
-  </si>
-  <si>
     <t>rstar_y_tf</t>
   </si>
   <si>
     <t>rstar_z_tf</t>
-  </si>
-  <si>
-    <t>tau_a</t>
-  </si>
-  <si>
-    <t>omega_moon</t>
-  </si>
-  <si>
-    <t>mu</t>
-  </si>
-  <si>
-    <t>rad/s</t>
-  </si>
-  <si>
-    <t>Moon rotation rate</t>
-  </si>
-  <si>
-    <t>m3/s2</t>
-  </si>
-  <si>
-    <t>Moon gravitational constant</t>
-  </si>
-  <si>
-    <t>km2m</t>
-  </si>
-  <si>
-    <t>errorPropTestEnable1</t>
   </si>
 </sst>
 </file>
@@ -857,14 +844,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1013,7 +999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1043,14 +1029,13 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1059,9 +1044,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1086,18 +1069,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1436,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1453,36 +1438,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="60" t="s">
+      <c r="B1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="58" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="59">
         <v>2</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="63">
+      <c r="E2" s="60">
         <f t="shared" ref="E2:E10" si="0">B2</f>
         <v>2</v>
       </c>
@@ -1491,7 +1476,7 @@
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="64">
+      <c r="B3" s="61">
         <v>0.25</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -1500,7 +1485,7 @@
       <c r="D3" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="65">
+      <c r="E3" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
@@ -1509,7 +1494,7 @@
       <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="64">
+      <c r="B4" s="61">
         <v>550</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -1518,7 +1503,7 @@
       <c r="D4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="62">
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
@@ -1527,7 +1512,7 @@
       <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="64">
+      <c r="B5" s="61">
         <f>2*PI()/SQRT(B9)*((B11+B12+2*B13)/2)^(3/2)</f>
         <v>6809.4202019908689</v>
       </c>
@@ -1537,7 +1522,7 @@
       <c r="D5" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="65">
+      <c r="E5" s="62">
         <f>B5</f>
         <v>6809.4202019908689</v>
       </c>
@@ -1546,7 +1531,7 @@
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="66">
+      <c r="B6" s="63">
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -1555,7 +1540,7 @@
       <c r="D6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="65">
+      <c r="E6" s="62">
         <f>B6</f>
         <v>3</v>
       </c>
@@ -1564,7 +1549,7 @@
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="66">
+      <c r="B7" s="63">
         <v>15</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -1573,7 +1558,7 @@
       <c r="D7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="65">
+      <c r="E7" s="62">
         <f>B7</f>
         <v>15</v>
       </c>
@@ -1582,7 +1567,7 @@
       <c r="A8" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="66">
+      <c r="B8" s="63">
         <f>12*6</f>
         <v>72</v>
       </c>
@@ -1592,7 +1577,7 @@
       <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="65">
+      <c r="E8" s="62">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
@@ -1601,7 +1586,7 @@
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="67">
+      <c r="B9" s="64">
         <v>4902.8010759999997</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1610,7 +1595,7 @@
       <c r="D9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="65">
+      <c r="E9" s="62">
         <f>B9*1000^3</f>
         <v>4902801076000</v>
       </c>
@@ -1619,7 +1604,7 @@
       <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="64">
+      <c r="B10" s="61">
         <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -1628,7 +1613,7 @@
       <c r="D10" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1637,7 +1622,7 @@
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="64">
+      <c r="B11" s="61">
         <v>100</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1646,7 +1631,7 @@
       <c r="D11" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="62">
         <f>B11*1000</f>
         <v>100000</v>
       </c>
@@ -1655,7 +1640,7 @@
       <c r="A12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="64">
+      <c r="B12" s="61">
         <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -1664,7 +1649,7 @@
       <c r="D12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="62">
         <f>B12*1000</f>
         <v>10000</v>
       </c>
@@ -1673,7 +1658,7 @@
       <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="64">
+      <c r="B13" s="61">
         <v>1737.4</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -1682,7 +1667,7 @@
       <c r="D13" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="62">
         <f>B13*1000</f>
         <v>1737400</v>
       </c>
@@ -1691,7 +1676,7 @@
       <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="64">
+      <c r="B14" s="61">
         <v>1737.4</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -1700,7 +1685,7 @@
       <c r="D14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="62">
         <f>B14*1000</f>
         <v>1737400</v>
       </c>
@@ -1709,7 +1694,7 @@
       <c r="A15" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="64">
+      <c r="B15" s="61">
         <v>13.17635815</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1718,7 +1703,7 @@
       <c r="D15" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="62">
         <f>RADIANS(B15)/86400</f>
         <v>2.6616994576329732E-6</v>
       </c>
@@ -1727,7 +1712,7 @@
       <c r="A16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="64">
+      <c r="B16" s="61">
         <v>0</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -1736,7 +1721,7 @@
       <c r="D16" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="62">
         <f>B16</f>
         <v>0</v>
       </c>
@@ -1745,7 +1730,7 @@
       <c r="A17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="64">
+      <c r="B17" s="61">
         <v>0</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -1754,7 +1739,7 @@
       <c r="D17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="62">
         <f>B17</f>
         <v>0</v>
       </c>
@@ -1763,7 +1748,7 @@
       <c r="A18" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="64">
+      <c r="B18" s="61">
         <v>0</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -1772,55 +1757,53 @@
       <c r="D18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="62">
         <f>B18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="B19" s="68">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
-      </c>
-      <c r="C19" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="65">
+        <v>55</v>
+      </c>
+      <c r="C19" s="64" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="E19" s="65">
+        <v>189</v>
+      </c>
+      <c r="E19" s="62">
         <f t="shared" ref="E19:E20" si="1">B19</f>
-        <v>3404.7101009954345</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="B20" s="68">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
-      </c>
-      <c r="C20" s="67" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20" s="65">
+        <v>55</v>
+      </c>
+      <c r="C20" s="64" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="62">
         <f t="shared" si="1"/>
-        <v>3404.7101009954345</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="66">
-        <v>0</v>
+      <c r="B21" s="63">
+        <v>1</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>4</v>
@@ -1828,388 +1811,392 @@
       <c r="D21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="65">
-        <f t="shared" ref="E21:E24" si="2">B21</f>
-        <v>0</v>
+      <c r="E21" s="62">
+        <f t="shared" ref="E21:E23" si="2">B21</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="B22" s="66">
+        <v>20</v>
+      </c>
+      <c r="B22" s="63">
         <v>1</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="65">
-        <f>B22</f>
+      <c r="C22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="62">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="66">
+        <v>36</v>
+      </c>
+      <c r="B23" s="63">
         <v>0</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="65">
+        <v>37</v>
+      </c>
+      <c r="E23" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="66">
-        <v>0</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="65">
-        <f t="shared" si="2"/>
+      <c r="A24" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" ref="E24:E26" si="3">RADIANS(B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="64">
-        <v>0</v>
-      </c>
-      <c r="C25" s="16" t="s">
+      <c r="A25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="65">
-        <f t="shared" ref="E25:E30" si="3">RADIANS(B25)</f>
+      <c r="D25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B26" s="64">
-        <v>0</v>
-      </c>
-      <c r="C26" s="16" t="s">
+      <c r="A26" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="2">
+        <v>180</v>
+      </c>
+      <c r="C26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E26" s="65">
+      <c r="D26" t="s">
+        <v>218</v>
+      </c>
+      <c r="E26" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.1415926535897931</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="64">
-        <v>180</v>
+      <c r="B27" s="61">
+        <v>0</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="65">
-        <f t="shared" si="3"/>
-        <v>3.1415926535897931</v>
+        <v>145</v>
+      </c>
+      <c r="E27" s="62">
+        <f t="shared" ref="E27:E29" si="4">RADIANS(B27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B28" s="64">
-        <v>0</v>
+        <v>143</v>
+      </c>
+      <c r="B28" s="61">
+        <v>-90</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E28" s="65">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>146</v>
+      </c>
+      <c r="E28" s="62">
+        <f t="shared" si="4"/>
+        <v>-1.5707963267948966</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="64">
-        <v>-90</v>
+        <v>144</v>
+      </c>
+      <c r="B29" s="61">
+        <v>30</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E29" s="65">
-        <f t="shared" si="3"/>
-        <v>-1.5707963267948966</v>
+        <v>147</v>
+      </c>
+      <c r="E29" s="62">
+        <f t="shared" si="4"/>
+        <v>0.52359877559829882</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="B30" s="64">
+        <v>139</v>
+      </c>
+      <c r="B30" s="61">
         <v>30</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E30" s="65">
-        <f t="shared" si="3"/>
-        <v>0.52359877559829882</v>
+        <v>165</v>
+      </c>
+      <c r="E30" s="62">
+        <f t="shared" ref="E30:E31" si="5">B30</f>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B31" s="64">
-        <v>30</v>
+        <v>141</v>
+      </c>
+      <c r="B31" s="61">
+        <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>140</v>
+        <v>4</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E31" s="65">
-        <f t="shared" ref="E31:E32" si="4">B31</f>
-        <v>30</v>
+        <v>164</v>
+      </c>
+      <c r="E31" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="64">
-        <v>0</v>
+        <v>155</v>
+      </c>
+      <c r="B32" s="61">
+        <v>19</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>4</v>
+        <v>157</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E32" s="65">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="E32" s="62">
+        <f>B32/1000</f>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" s="61">
+        <v>7</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="64">
-        <v>19</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="E33" s="65">
-        <f>B33/1000</f>
-        <v>1.9E-2</v>
+      <c r="E33" s="62">
+        <f>B33*0.000001</f>
+        <v>6.9999999999999999E-6</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B34" s="64">
-        <v>7</v>
+        <v>158</v>
+      </c>
+      <c r="B34" s="61">
+        <v>2500</v>
       </c>
       <c r="C34" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E34" s="65">
-        <f>B34*0.000001</f>
-        <v>6.9999999999999999E-6</v>
+      <c r="E34" s="62">
+        <f t="shared" ref="E34:E35" si="6">B34</f>
+        <v>2500</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="64">
+        <v>159</v>
+      </c>
+      <c r="B35" s="61">
         <v>2500</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>134</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="65">
-        <f t="shared" ref="E35:E36" si="5">B35</f>
+        <v>163</v>
+      </c>
+      <c r="E35" s="62">
+        <f t="shared" si="6"/>
         <v>2500</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="64">
-        <v>2500</v>
+        <v>167</v>
+      </c>
+      <c r="B36" s="63">
+        <v>5</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="D36" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="62">
+        <f>B36</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="48">
+        <v>1</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="50">
+        <f t="shared" ref="E37:E39" si="7">B37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="52">
+        <v>1</v>
+      </c>
+      <c r="C38" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="54">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="68">
+        <v>0</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="65">
-        <f t="shared" si="5"/>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
+      <c r="E39" s="60">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" s="63">
+        <v>0</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="62">
+        <f t="shared" ref="E40" si="8">B40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B37" s="66">
-        <v>5</v>
-      </c>
-      <c r="C37" s="16" t="s">
+      <c r="B41" s="66">
+        <v>0</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E37" s="65">
-        <f>B37</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="50" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="51">
-        <v>1</v>
-      </c>
-      <c r="C38" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="53">
-        <f t="shared" ref="E38:E40" si="6">B38</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="55">
-        <v>1</v>
-      </c>
-      <c r="C39" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="E39" s="57">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" s="71">
-        <v>0</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="63">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="B41" s="66">
-        <v>0</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E41" s="65">
-        <f t="shared" ref="E41" si="7">B41</f>
+      <c r="E41" s="67">
+        <f t="shared" ref="E41:E54" si="9">B41</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B42" s="69">
-        <v>0</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" s="70">
-        <f t="shared" ref="E42:E51" si="8">B42</f>
-        <v>0</v>
+      <c r="A42" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1737.5</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E42" s="1">
+        <f>B42*1000</f>
+        <v>1737500</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="B43" s="2">
         <v>1737.5</v>
@@ -2218,233 +2205,210 @@
         <v>52</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="8"/>
-        <v>1737.5</v>
+        <f>B43*1000</f>
+        <v>1737500</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>234</v>
+      <c r="A44" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="B44" s="2">
-        <v>1737.5</v>
+        <v>0</v>
       </c>
       <c r="C44" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="9"/>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="8"/>
-        <v>1737.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B45" s="2">
-        <v>0</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1.62</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="E46" s="1">
-        <f t="shared" si="8"/>
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B47" s="2">
-        <v>0</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="E47" s="1">
-        <f t="shared" ref="E47" si="9">B47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="E48" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="B49" s="2">
-        <v>-1</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E49" s="1">
-        <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="B50" s="2">
-        <v>0</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>243</v>
-      </c>
       <c r="D50" s="16" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" ref="E50" si="10">B50</f>
+        <f>B50*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
-        <v>245</v>
+      <c r="A51" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="B51" s="2">
-        <v>0</v>
+        <v>1738</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" ref="E51:E52" si="10">B51*1000</f>
+        <v>1738000</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
-        <v>249</v>
+      <c r="A52" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="B52" s="2">
-        <v>1738</v>
+        <v>0</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="E52" s="1">
-        <f>B52*1000</f>
-        <v>1738000</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="B53" s="2">
-        <v>0</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>52</v>
+      <c r="A53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" s="80">
+        <v>2.7E-6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>205</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" ref="E53:E55" si="11">B53</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>2.7E-6</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="B54" s="82">
-        <v>2.7E-6</v>
+      <c r="A54" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="81">
+        <v>4904869500000</v>
       </c>
       <c r="C54" t="s">
-        <v>254</v>
-      </c>
-      <c r="D54" t="s">
-        <v>255</v>
+        <v>207</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="11"/>
-        <v>2.7E-6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="B55" s="83">
+        <f t="shared" si="9"/>
         <v>4904869500000</v>
       </c>
-      <c r="C55" t="s">
-        <v>256</v>
-      </c>
-      <c r="D55" t="s">
-        <v>257</v>
-      </c>
-      <c r="E55" s="1">
-        <f t="shared" si="11"/>
-        <v>4904869500000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2454,15 +2418,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2500,47 +2465,39 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>258</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="23" t="s">
@@ -2549,34 +2506,33 @@
       <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="73" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="31">
         <v>-390</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="31">
-        <f>B2*km2m</f>
+      <c r="E2" s="74">
+        <f>B2*1000</f>
         <v>-390000</v>
       </c>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="33">
         <f>10.3957+1737.5</f>
         <v>1747.8957</v>
       </c>
@@ -2586,13 +2542,13 @@
       <c r="D3" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="31">
-        <f>B3*km2m</f>
+      <c r="E3" s="74">
+        <f>B3*1000</f>
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="35">
@@ -2604,49 +2560,49 @@
       <c r="D4" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="36">
-        <f>B4*km2m</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="E4" s="75">
+        <f t="shared" ref="E4" si="0">B4*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="33">
         <v>1.7</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="31">
-        <f t="shared" ref="E5:E23" si="0">B5*1000</f>
+      <c r="E5" s="74">
+        <f>B5*1000</f>
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="33">
         <v>0</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>78</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="E6" s="74">
+        <f>B6*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="33">
@@ -2658,278 +2614,296 @@
       <c r="D7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="81" t="s">
-        <v>214</v>
-      </c>
-      <c r="B8" s="27">
+      <c r="E7" s="74">
+        <f>B7*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="44">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="76">
+        <f>B8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="29">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="76">
+        <f t="shared" ref="E9:E19" si="1">B9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="69">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E8" s="12">
-        <f t="shared" ref="E8:E15" si="1">B8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" s="15">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E10" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="B11" s="15">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="B12" s="27">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="77">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="78">
+        <f>B12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" s="69">
+        <v>0</v>
+      </c>
+      <c r="C13" s="16">
         <v>0</v>
       </c>
       <c r="D13" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" s="69">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" s="28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="E13" s="13">
+      <c r="B16" s="72">
+        <v>0</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="79">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="B14" s="15">
-        <v>0</v>
-      </c>
-      <c r="D14" s="16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="13">
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="78">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="80" t="s">
-        <v>221</v>
-      </c>
-      <c r="B15" s="20">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>229</v>
       </c>
-      <c r="E15" s="14">
+      <c r="B18" s="16">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" s="74">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="E16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="B17" s="75">
-        <v>0</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E17" s="65">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="B18" s="75">
-        <v>0</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="E18" s="65">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B19" s="74">
-        <v>0</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="70">
-        <f t="shared" si="0"/>
+      <c r="E19" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="72">
+        <v>0</v>
+      </c>
+      <c r="C20" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="B20" s="74">
-        <v>0</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="E20" s="70">
-        <f t="shared" si="0"/>
+      <c r="E20" s="78">
+        <f>B20*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B21" s="75">
-        <v>0</v>
-      </c>
-      <c r="C21" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" s="65">
-        <f t="shared" si="0"/>
+      <c r="E21" s="78">
+        <f>B21</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="16">
+        <v>0</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="75">
-        <v>0</v>
-      </c>
-      <c r="C22" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D22" t="s">
-        <v>195</v>
-      </c>
-      <c r="E22" s="65">
-        <f t="shared" si="0"/>
+      <c r="E22" s="78">
+        <f t="shared" ref="E22:E23" si="2">B22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="B23" s="74">
-        <v>0</v>
-      </c>
-      <c r="C23" s="77" t="s">
-        <v>193</v>
+        <v>234</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" s="70">
-        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="E23" s="78">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2944,7 +2918,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3007,7 +2981,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3024,7 +2998,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>236</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -3041,7 +3015,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -3075,7 +3049,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -3092,7 +3066,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -3112,14 +3086,12 @@
         <v>38</v>
       </c>
       <c r="B10">
-        <f>B2</f>
         <v>1</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10">
-        <f>D2</f>
         <v>1</v>
       </c>
       <c r="E10">
@@ -3140,7 +3112,7 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3153,7 +3125,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3216,7 +3188,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3250,7 +3222,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -3267,7 +3239,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3327,11 +3299,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3344,19 +3314,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3507,20 +3477,20 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="45" t="s">
         <v>135</v>
       </c>
       <c r="B10" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="46" t="s">
         <v>138</v>
       </c>
       <c r="E10" s="12">
-        <f t="shared" ref="E10:E14" si="1">B10/3</f>
+        <f>B10/3</f>
         <v>1</v>
       </c>
     </row>
@@ -3538,13 +3508,13 @@
         <v>137</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" si="1"/>
+        <f>B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B12" s="9">
         <v>10</v>
@@ -3553,16 +3523,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f>B12/3</f>
         <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B13" s="9">
         <v>100</v>
@@ -3571,16 +3541,16 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f>B13/3</f>
         <v>33.333333333333336</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B14" s="9">
         <v>10</v>
@@ -3589,30 +3559,12 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f>B14/3</f>
         <v>3.3333333333333335</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4012,19 +3964,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4209,7 +4161,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="str">
+      <c r="A10" s="45" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
@@ -4217,11 +4169,11 @@
         <f>truthStateParams!B10</f>
         <v>3</v>
       </c>
-      <c r="C10" s="49" t="str">
+      <c r="C10" s="46" t="str">
         <f>truthStateParams!C10</f>
         <v>pixels</v>
       </c>
-      <c r="D10" s="49" t="str">
+      <c r="D10" s="46" t="str">
         <f>truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
@@ -4343,16 +4295,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
@@ -4376,7 +4328,7 @@
         <f>truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="41">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
         <v>1333.3333333333333</v>
       </c>
@@ -4399,7 +4351,7 @@
         <f>truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
@@ -4422,7 +4374,7 @@
         <f>truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="41">
         <f t="shared" si="0"/>
         <v>1333.3333333333333</v>
       </c>
@@ -4445,7 +4397,7 @@
         <f>truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4468,7 +4420,7 @@
         <f>truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4490,7 +4442,7 @@
         <f>truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4512,7 +4464,7 @@
         <f>truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
@@ -4534,7 +4486,7 @@
         <f>truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
@@ -4556,7 +4508,7 @@
         <f>truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
@@ -4578,7 +4530,7 @@
         <f>truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="41">
         <f>RADIANS(B11)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4600,7 +4552,7 @@
         <f>truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="41">
         <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4622,7 +4574,7 @@
         <f>truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4644,7 +4596,7 @@
         <f>truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4666,7 +4618,7 @@
         <f>truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4688,7 +4640,7 @@
         <f>truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="41">
         <f t="shared" si="1"/>
         <v>3.2320912073969067E-5</v>
       </c>
@@ -4710,7 +4662,7 @@
         <f>truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="41">
         <f>RADIANS(B17)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4732,7 +4684,7 @@
         <f>truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="41">
         <f>RADIANS(B18)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4754,7 +4706,7 @@
         <f>truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="42">
         <f>RADIANS(B19)/hr2sec/3</f>
         <v>8.0802280184922667E-6</v>
       </c>
@@ -4767,38 +4719,40 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>116</v>
       </c>
@@ -4812,13 +4766,13 @@
       <c r="D2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="70">
         <f t="shared" ref="E2:E7" si="0">B2</f>
         <v>100</v>
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>117</v>
       </c>
@@ -4832,33 +4786,33 @@
       <c r="D3" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="70">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>300</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="6" t="str">
         <f>truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="70">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>119</v>
       </c>
@@ -4872,13 +4826,13 @@
       <c r="D5" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="70">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -4892,225 +4846,339 @@
       <c r="D6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="70">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="str">
+      <c r="C7" s="6" t="str">
         <f>truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="70">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="78" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="76">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="82" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="6">
         <v>10</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="76" t="s">
-        <v>209</v>
-      </c>
-      <c r="E8" s="79">
-        <f>B8/1000</f>
-        <v>0.01</v>
+      <c r="D8" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="70">
+        <f>B8</f>
+        <v>10</v>
       </c>
       <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
+        <v>240</v>
+      </c>
+      <c r="B9" s="26">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="70">
+        <f t="shared" ref="E9:E15" si="1">B9</f>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="26">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="70">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="26">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="70">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="82" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="16">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="70">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="16">
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E9" s="42">
-        <f>B9/1000</f>
-        <v>1E-3</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="D13" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="70">
+        <f t="shared" si="1"/>
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="16">
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E10" s="42">
-        <f>B10/1000</f>
-        <v>2E-3</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" s="8">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="D14" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E14" s="70">
+        <f t="shared" si="1"/>
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="17">
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="E11" s="43">
-        <f t="shared" ref="E11:E15" si="1">RADIANS(B11)/3600</f>
-        <v>1.454441043328608E-5</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="78" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="76">
-        <v>10</v>
-      </c>
-      <c r="C12" s="76" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="76" t="s">
-        <v>211</v>
-      </c>
-      <c r="E12" s="79">
+      <c r="D15" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="71">
         <f t="shared" si="1"/>
-        <v>4.8481368110953597E-5</v>
-      </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" s="42">
-        <f t="shared" si="1"/>
-        <v>4.8481368110953598E-6</v>
-      </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E14" s="42">
-        <f t="shared" si="1"/>
-        <v>4.8481368110953598E-6</v>
-      </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="C15" s="77" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="43">
-        <f t="shared" si="1"/>
-        <v>4.8481368110953598E-6</v>
+        <v>3.2699999999999999E-3</v>
       </c>
       <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the covariance propagation
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A75E1D7-579C-CC4F-BC53-B40ADBD05393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7271014-5A80-8846-A5EE-19D443EE36A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="242">
   <si>
     <t>Value</t>
   </si>
@@ -78,9 +78,6 @@
     <t>rad</t>
   </si>
   <si>
-    <t>deg/sqrt(hr)</t>
-  </si>
-  <si>
     <t>3-sigma angular random walk</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>number of "model replacement" measurements</t>
   </si>
   <si>
-    <t>arw</t>
-  </si>
-  <si>
     <t>hrs2min</t>
   </si>
   <si>
@@ -120,12 +114,6 @@
     <t>dt</t>
   </si>
   <si>
-    <t>sig_gyro_ss</t>
-  </si>
-  <si>
-    <t>deg/hr</t>
-  </si>
-  <si>
     <t>3-sigma steady-state gyro bias</t>
   </si>
   <si>
@@ -291,18 +279,12 @@
     <t>vi_z</t>
   </si>
   <si>
-    <t>arcsec/axis</t>
-  </si>
-  <si>
     <t>3-sigma steady-state star camera misalignment</t>
   </si>
   <si>
     <t>3-sigma steady-state terrain camera misalignment</t>
   </si>
   <si>
-    <t>arcsec</t>
-  </si>
-  <si>
     <t>3-sigma star camera measurement uncertainty</t>
   </si>
   <si>
@@ -336,39 +318,6 @@
     <t>3-sigma initial satellite orientation uncertainty</t>
   </si>
   <si>
-    <t>3-sigma initial star camera misalignment uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial terrain camera misalignment uncertainty</t>
-  </si>
-  <si>
-    <t>sig_gyrox</t>
-  </si>
-  <si>
-    <t>3-sigma initial gyro bias uncertainty</t>
-  </si>
-  <si>
-    <t>sig_gyroy</t>
-  </si>
-  <si>
-    <t>sig_gyroz</t>
-  </si>
-  <si>
-    <t>sig_st_ss</t>
-  </si>
-  <si>
-    <t>sig_c_ss</t>
-  </si>
-  <si>
-    <t>sig_meas_stx</t>
-  </si>
-  <si>
-    <t>sig_meas_sty</t>
-  </si>
-  <si>
-    <t>sig_meas_stz</t>
-  </si>
-  <si>
     <t>sig_ax</t>
   </si>
   <si>
@@ -378,24 +327,6 @@
     <t>sig_az</t>
   </si>
   <si>
-    <t>sig_thcx</t>
-  </si>
-  <si>
-    <t>sig_thcy</t>
-  </si>
-  <si>
-    <t>sig_thcz</t>
-  </si>
-  <si>
-    <t>sig_thstx</t>
-  </si>
-  <si>
-    <t>sig_thsty</t>
-  </si>
-  <si>
-    <t>sig_thstz</t>
-  </si>
-  <si>
     <t>del_rsx</t>
   </si>
   <si>
@@ -420,9 +351,6 @@
     <t>MatlabValues</t>
   </si>
   <si>
-    <t>processStarTrackerEnable</t>
-  </si>
-  <si>
     <t>processVisualOdometryEnable</t>
   </si>
   <si>
@@ -435,36 +363,18 @@
     <t>n_MonteCarloRuns</t>
   </si>
   <si>
-    <t>Q_grav</t>
-  </si>
-  <si>
     <t>m^2/s^3</t>
   </si>
   <si>
     <t>3-sigma non-gravitational process noise</t>
   </si>
   <si>
-    <t>flag to enable processing of star camera measurements</t>
-  </si>
-  <si>
     <t>flag to enable processing of VO measurements</t>
   </si>
   <si>
     <t>pixels</t>
   </si>
   <si>
-    <t>sig_cu</t>
-  </si>
-  <si>
-    <t>sig_cv</t>
-  </si>
-  <si>
-    <t>3-sigma v component of pixel noise</t>
-  </si>
-  <si>
-    <t>3-sigma u component of pixel noise</t>
-  </si>
-  <si>
     <t>n_features</t>
   </si>
   <si>
@@ -492,24 +402,6 @@
     <t>x angle of a ZYX euler angle sequence to define C orientation wrt body</t>
   </si>
   <si>
-    <t>sig_idpos</t>
-  </si>
-  <si>
-    <t>3-sigma change in inertial position measurement uncertainty</t>
-  </si>
-  <si>
-    <t>sig_loss</t>
-  </si>
-  <si>
-    <t>3-sigma LOSS feature location uncertainty</t>
-  </si>
-  <si>
-    <t>sig_mdpos</t>
-  </si>
-  <si>
-    <t>3-sigma change in lunar-referenced position measurement uncertainty</t>
-  </si>
-  <si>
     <t>days2hrs</t>
   </si>
   <si>
@@ -687,24 +579,6 @@
     <t>m/s4</t>
   </si>
   <si>
-    <t>thz_st</t>
-  </si>
-  <si>
-    <t>z angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
-    <t>thy_st</t>
-  </si>
-  <si>
-    <t>y angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
-    <t>thx_st</t>
-  </si>
-  <si>
-    <t>x angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
     <t>qm_i_a</t>
   </si>
   <si>
@@ -814,6 +688,90 @@
   </si>
   <si>
     <t>rstar_z_tf</t>
+  </si>
+  <si>
+    <t>Q_nongrav</t>
+  </si>
+  <si>
+    <t>sig_rbias_ss</t>
+  </si>
+  <si>
+    <t>sig_abias_ss</t>
+  </si>
+  <si>
+    <t>sig_grav_ss</t>
+  </si>
+  <si>
+    <t>sig_h_ss</t>
+  </si>
+  <si>
+    <t>vrw</t>
+  </si>
+  <si>
+    <t>m/s^2</t>
+  </si>
+  <si>
+    <t>m/s/sqrt(hr)</t>
+  </si>
+  <si>
+    <t>sig_epsx</t>
+  </si>
+  <si>
+    <t>3-sigma gravity bias uncertainty</t>
+  </si>
+  <si>
+    <t>sig_epsy</t>
+  </si>
+  <si>
+    <t>sig_epsz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma lander height uncertainty </t>
+  </si>
+  <si>
+    <t>sig_h</t>
+  </si>
+  <si>
+    <t>sig_br</t>
+  </si>
+  <si>
+    <t>Random walk for the velocity</t>
+  </si>
+  <si>
+    <t>3-sigma height bias uncertainty at steady state</t>
+  </si>
+  <si>
+    <t>3-sigma gravity bias uncertainty at steady state</t>
+  </si>
+  <si>
+    <t>3-sigma accleromenter bias uncertainty at steady state</t>
+  </si>
+  <si>
+    <t>3-sigma range bias uncertainty at steady state</t>
+  </si>
+  <si>
+    <t>sig_rx</t>
+  </si>
+  <si>
+    <t>sig_ry</t>
+  </si>
+  <si>
+    <t>sig_rz</t>
+  </si>
+  <si>
+    <t>sig_vx</t>
+  </si>
+  <si>
+    <t>sig_vy</t>
+  </si>
+  <si>
+    <t>sig_vz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma acclerometer bias uncertatintiy </t>
+  </si>
+  <si>
+    <t>3-sigma initial range bias uncertainty</t>
   </si>
 </sst>
 </file>
@@ -826,7 +784,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,6 +813,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -870,7 +835,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -995,11 +960,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1019,15 +1011,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1042,7 +1031,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1051,10 +1039,6 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1083,6 +1067,11 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:A52"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1438,81 +1427,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="58" t="s">
-        <v>123</v>
+      <c r="E1" s="50" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="51">
         <v>2</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="60">
+      <c r="E2" s="52">
         <f t="shared" ref="E2:E10" si="0">B2</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="61">
+        <v>21</v>
+      </c>
+      <c r="B3" s="53">
         <v>0.25</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="62">
+        <v>50</v>
+      </c>
+      <c r="E3" s="54">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="61">
+        <v>36</v>
+      </c>
+      <c r="B4" s="53">
         <v>550</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="62">
+        <v>51</v>
+      </c>
+      <c r="E4" s="54">
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="61">
+        <v>37</v>
+      </c>
+      <c r="B5" s="53">
         <f>2*PI()/SQRT(B9)*((B11+B12+2*B13)/2)^(3/2)</f>
         <v>6809.4202019908689</v>
       </c>
@@ -1520,54 +1509,54 @@
         <v>5</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="62">
+        <v>52</v>
+      </c>
+      <c r="E5" s="54">
         <f>B5</f>
         <v>6809.4202019908689</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="63">
+        <v>11</v>
+      </c>
+      <c r="B6" s="55">
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="62">
+        <v>13</v>
+      </c>
+      <c r="E6" s="54">
         <f>B6</f>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="63">
+        <v>53</v>
+      </c>
+      <c r="B7" s="55">
         <v>15</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="62">
+        <v>54</v>
+      </c>
+      <c r="E7" s="54">
         <f>B7</f>
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="63">
+        <v>104</v>
+      </c>
+      <c r="B8" s="55">
         <f>12*6</f>
         <v>72</v>
       </c>
@@ -1575,838 +1564,766 @@
         <v>4</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="62">
+        <v>12</v>
+      </c>
+      <c r="E8" s="54">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="64">
+        <v>38</v>
+      </c>
+      <c r="B9" s="56">
         <v>4902.8010759999997</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="62">
+        <v>55</v>
+      </c>
+      <c r="E9" s="54">
         <f>B9*1000^3</f>
         <v>4902801076000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="61">
+        <v>39</v>
+      </c>
+      <c r="B10" s="53">
         <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="62">
+        <v>56</v>
+      </c>
+      <c r="E10" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="61">
+        <v>40</v>
+      </c>
+      <c r="B11" s="53">
         <v>100</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="62">
+        <v>57</v>
+      </c>
+      <c r="E11" s="54">
         <f>B11*1000</f>
         <v>100000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="61">
+        <v>41</v>
+      </c>
+      <c r="B12" s="53">
         <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="62">
+        <v>58</v>
+      </c>
+      <c r="E12" s="54">
         <f>B12*1000</f>
         <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="61">
+        <v>42</v>
+      </c>
+      <c r="B13" s="53">
         <v>1737.4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="62">
+        <v>59</v>
+      </c>
+      <c r="E13" s="54">
         <f>B13*1000</f>
         <v>1737400</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="61">
+        <v>43</v>
+      </c>
+      <c r="B14" s="53">
         <v>1737.4</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="62">
+        <v>60</v>
+      </c>
+      <c r="E14" s="54">
         <f>B14*1000</f>
         <v>1737400</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="61">
+        <v>99</v>
+      </c>
+      <c r="B15" s="53">
         <v>13.17635815</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="62">
+        <v>61</v>
+      </c>
+      <c r="E15" s="54">
         <f>RADIANS(B15)/86400</f>
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="61">
+        <v>44</v>
+      </c>
+      <c r="B16" s="53">
         <v>0</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="62">
+        <v>62</v>
+      </c>
+      <c r="E16" s="54">
         <f>B16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="61">
+        <v>45</v>
+      </c>
+      <c r="B17" s="53">
         <v>0</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="62">
+        <v>63</v>
+      </c>
+      <c r="E17" s="54">
         <f>B17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="61">
+        <v>46</v>
+      </c>
+      <c r="B18" s="53">
         <v>0</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="62">
+        <v>64</v>
+      </c>
+      <c r="E18" s="54">
         <f>B18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="B19" s="65">
+        <v>152</v>
+      </c>
+      <c r="B19" s="57">
         <v>55</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="56" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E19" s="62">
+        <v>153</v>
+      </c>
+      <c r="E19" s="54">
         <f t="shared" ref="E19:E20" si="1">B19</f>
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B20" s="65">
+        <v>173</v>
+      </c>
+      <c r="B20" s="57">
         <v>55</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C20" s="56" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="62">
+        <v>65</v>
+      </c>
+      <c r="E20" s="54">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="63">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B21" s="55">
+        <v>0</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="62">
+        <v>31</v>
+      </c>
+      <c r="E21" s="54">
         <f t="shared" ref="E21:E23" si="2">B21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="63">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="55">
+        <v>0</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="62">
+        <v>19</v>
+      </c>
+      <c r="E22" s="54">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="63">
+        <v>32</v>
+      </c>
+      <c r="B23" s="55">
         <v>0</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="62">
+        <v>33</v>
+      </c>
+      <c r="E23" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>214</v>
-      </c>
-      <c r="E24" s="13">
+      <c r="A24" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="53">
+        <v>0</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="54">
         <f t="shared" ref="E24:E26" si="3">RADIANS(B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" t="s">
-        <v>216</v>
-      </c>
-      <c r="E25" s="13">
+      <c r="A25" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="53">
+        <v>-90</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="54">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1.5707963267948966</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B26" s="2">
-        <v>180</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>218</v>
-      </c>
-      <c r="E26" s="13">
+      <c r="A26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="53">
+        <v>30</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="54">
         <f t="shared" si="3"/>
-        <v>3.1415926535897931</v>
+        <v>0.52359877559829882</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B27" s="61">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="B27" s="53">
+        <v>30</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="62">
-        <f t="shared" ref="E27:E29" si="4">RADIANS(B27)</f>
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="E27" s="54">
+        <f t="shared" ref="E27:E28" si="4">B27</f>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="61">
-        <v>-90</v>
+        <v>111</v>
+      </c>
+      <c r="B28" s="53">
+        <v>0</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E28" s="62">
+        <v>128</v>
+      </c>
+      <c r="E28" s="54">
         <f t="shared" si="4"/>
-        <v>-1.5707963267948966</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" s="61">
-        <v>30</v>
+        <v>119</v>
+      </c>
+      <c r="B29" s="53">
+        <v>19</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E29" s="62">
-        <f t="shared" si="4"/>
-        <v>0.52359877559829882</v>
+        <v>124</v>
+      </c>
+      <c r="E29" s="54">
+        <f>B29/1000</f>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="61">
-        <v>30</v>
+        <v>130</v>
+      </c>
+      <c r="B30" s="53">
+        <v>7</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="E30" s="62">
-        <f t="shared" ref="E30:E31" si="5">B30</f>
-        <v>30</v>
+        <v>125</v>
+      </c>
+      <c r="E30" s="54">
+        <f>B30*0.000001</f>
+        <v>6.9999999999999999E-6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="61">
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="B31" s="53">
+        <v>2500</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="62">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>126</v>
+      </c>
+      <c r="E31" s="54">
+        <f t="shared" ref="E31:E32" si="5">B31</f>
+        <v>2500</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" s="61">
-        <v>19</v>
+        <v>123</v>
+      </c>
+      <c r="B32" s="53">
+        <v>2500</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="E32" s="62">
-        <f>B32/1000</f>
-        <v>1.9E-2</v>
+        <v>127</v>
+      </c>
+      <c r="E32" s="54">
+        <f t="shared" si="5"/>
+        <v>2500</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B33" s="61">
-        <v>7</v>
+        <v>131</v>
+      </c>
+      <c r="B33" s="55">
+        <v>5</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>156</v>
+        <v>4</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="E33" s="62">
-        <f>B33*0.000001</f>
-        <v>6.9999999999999999E-6</v>
+        <v>132</v>
+      </c>
+      <c r="E33" s="54">
+        <f>B33</f>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="61">
-        <v>2500</v>
-      </c>
-      <c r="C34" s="16" t="s">
+      <c r="A34" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="44">
+        <v>0</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="46">
+        <f t="shared" ref="E34:E35" si="6">B34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E34" s="62">
-        <f t="shared" ref="E34:E35" si="6">B34</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="B35" s="61">
-        <v>2500</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E35" s="62">
+      <c r="B35" s="60">
+        <v>0</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="52">
         <f t="shared" si="6"/>
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="B36" s="63">
-        <v>5</v>
+        <v>135</v>
+      </c>
+      <c r="B36" s="55">
+        <v>0</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="62">
-        <f>B36</f>
-        <v>5</v>
+        <v>136</v>
+      </c>
+      <c r="E36" s="54">
+        <f t="shared" ref="E36" si="7">B36</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="48">
-        <v>1</v>
-      </c>
-      <c r="C37" s="49" t="s">
+      <c r="A37" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="58">
+        <v>0</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="50">
-        <f t="shared" ref="E37:E39" si="7">B37</f>
-        <v>1</v>
+      <c r="D37" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="59">
+        <f t="shared" ref="E37:E50" si="8">B37</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="B38" s="52">
-        <v>1</v>
-      </c>
-      <c r="C38" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="E38" s="54">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="A38" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1737.5</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" s="1">
+        <f>B38*1000</f>
+        <v>1737500</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="B39" s="68">
-        <v>0</v>
-      </c>
-      <c r="C39" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="46" t="s">
-        <v>169</v>
-      </c>
-      <c r="E39" s="60">
-        <f t="shared" si="7"/>
-        <v>0</v>
+      <c r="A39" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1737.5</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" s="1">
+        <f>B39*1000</f>
+        <v>1737500</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" s="63">
+      <c r="A40" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" s="2">
         <v>0</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="62">
-        <f t="shared" ref="E40" si="8">B40</f>
+        <v>160</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B41" s="66">
-        <v>0</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E41" s="67">
-        <f t="shared" ref="E41:E54" si="9">B41</f>
-        <v>0</v>
+      <c r="A41" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="8"/>
+        <v>1.62</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>190</v>
+      <c r="A42" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="B42" s="2">
-        <v>1737.5</v>
+        <v>0</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="E42" s="1">
-        <f>B42*1000</f>
-        <v>1737500</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>192</v>
+      <c r="A43" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="B43" s="2">
-        <v>1737.5</v>
+        <v>0</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="E43" s="1">
-        <f>B43*1000</f>
-        <v>1737500</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
       <c r="B44" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="B45" s="2">
-        <v>1.62</v>
+        <v>0</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="9"/>
-        <v>1.62</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="B46" s="2">
         <v>0</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>194</v>
+        <v>48</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="9"/>
+        <f>B46*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="B47" s="2">
-        <v>0</v>
+        <v>1738</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>195</v>
+        <v>48</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" ref="E47:E48" si="9">B47*1000</f>
+        <v>1738000</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="B48" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>195</v>
+        <v>48</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>195</v>
+      <c r="A49" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" s="72">
+        <v>2.7E-6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>169</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2.7E-6</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B50" s="2">
-        <v>0</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>52</v>
+      <c r="A50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="73">
+        <v>4904869500000</v>
+      </c>
+      <c r="C50" t="s">
+        <v>171</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="E50" s="1">
-        <f>B50*1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1738</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E51" s="1">
-        <f t="shared" ref="E51:E52" si="10">B51*1000</f>
-        <v>1738000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B52" s="2">
-        <v>0</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E52" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>203</v>
-      </c>
-      <c r="B53" s="80">
-        <v>2.7E-6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>205</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="E53" s="1">
-        <f t="shared" si="9"/>
-        <v>2.7E-6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>204</v>
-      </c>
-      <c r="B54" s="81">
-        <v>4904869500000</v>
-      </c>
-      <c r="C54" t="s">
-        <v>207</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="E54" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>4904869500000</v>
       </c>
     </row>
@@ -2432,7 +2349,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <v>60</v>
@@ -2440,7 +2357,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>60</v>
@@ -2448,7 +2365,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>hr2min*min2sec</f>
@@ -2457,7 +2374,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>9.81</v>
@@ -2465,7 +2382,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2481,7 +2398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -2490,192 +2407,192 @@
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="73" t="s">
-        <v>123</v>
+      <c r="E1" s="65" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="31">
+        <v>67</v>
+      </c>
+      <c r="B2" s="28">
         <v>-390</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="74">
+      <c r="C2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="66">
         <f>B2*1000</f>
         <v>-390000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="33">
+        <v>69</v>
+      </c>
+      <c r="B3" s="30">
         <f>10.3957+1737.5</f>
         <v>1747.8957</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="74">
+      <c r="C3" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="66">
         <f>B3*1000</f>
         <v>1747895.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="35">
-        <v>0</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="75">
+        <v>71</v>
+      </c>
+      <c r="B4" s="32">
+        <v>0</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="67">
         <f t="shared" ref="E4" si="0">B4*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="33">
+        <v>73</v>
+      </c>
+      <c r="B5" s="30">
         <v>1.7</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="74">
+      <c r="C5" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="66">
         <f>B5*1000</f>
         <v>1700</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="33">
-        <v>0</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="30">
+        <v>0</v>
+      </c>
+      <c r="C6" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="74">
+      <c r="D6" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="66">
         <f>B6*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="33">
-        <v>0</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="74">
+      <c r="B7" s="30">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="66">
         <f>B7*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B8" s="44">
+        <v>177</v>
+      </c>
+      <c r="B8" s="40">
         <v>0</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="76">
+        <v>139</v>
+      </c>
+      <c r="E8" s="68">
         <f>B8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>220</v>
-      </c>
-      <c r="B9" s="29">
+        <v>178</v>
+      </c>
+      <c r="B9" s="26">
         <v>0</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="76">
+        <v>139</v>
+      </c>
+      <c r="E9" s="68">
         <f t="shared" ref="E9:E19" si="1">B9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>221</v>
-      </c>
-      <c r="B10" s="69">
+        <v>179</v>
+      </c>
+      <c r="B10" s="61">
         <v>0</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" s="76">
+        <v>139</v>
+      </c>
+      <c r="E10" s="68">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -2684,16 +2601,16 @@
         <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" s="77">
+        <v>139</v>
+      </c>
+      <c r="E11" s="69">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -2702,52 +2619,52 @@
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E12" s="78">
+        <v>144</v>
+      </c>
+      <c r="E12" s="70">
         <f>B12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>224</v>
-      </c>
-      <c r="B13" s="69">
+        <v>182</v>
+      </c>
+      <c r="B13" s="61">
         <v>0</v>
       </c>
       <c r="C13" s="16">
         <v>0</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="E13" s="64">
+        <v>144</v>
+      </c>
+      <c r="E13" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>225</v>
-      </c>
-      <c r="B14" s="69">
+        <v>183</v>
+      </c>
+      <c r="B14" s="61">
         <v>0</v>
       </c>
       <c r="C14" s="16">
         <v>0</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="E14" s="64">
+        <v>144</v>
+      </c>
+      <c r="E14" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -2756,34 +2673,34 @@
         <v>0</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E15" s="28">
+        <v>144</v>
+      </c>
+      <c r="E15" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B16" s="72">
-        <v>0</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="79">
+        <v>185</v>
+      </c>
+      <c r="B16" s="64">
+        <v>0</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="71">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -2792,16 +2709,16 @@
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E17" s="78">
+        <v>146</v>
+      </c>
+      <c r="E17" s="70">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -2810,16 +2727,16 @@
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E18" s="26">
+        <v>147</v>
+      </c>
+      <c r="E18" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="B19" s="8">
         <v>0</v>
@@ -2828,34 +2745,34 @@
         <v>0</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E19" s="28">
+        <v>148</v>
+      </c>
+      <c r="E19" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B20" s="72">
-        <v>0</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="72" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" s="78">
+        <v>189</v>
+      </c>
+      <c r="B20" s="64">
+        <v>0</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="70">
         <f>B20*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
@@ -2864,16 +2781,16 @@
         <v>0</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E21" s="78">
+        <v>150</v>
+      </c>
+      <c r="E21" s="70">
         <f>B21</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="B22" s="16">
         <v>0</v>
@@ -2882,16 +2799,16 @@
         <v>0</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="E22" s="78">
+        <v>151</v>
+      </c>
+      <c r="E22" s="70">
         <f t="shared" ref="E22:E23" si="2">B22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="B23" s="8">
         <v>0</v>
@@ -2900,9 +2817,9 @@
         <v>0</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E23" s="78">
+        <v>151</v>
+      </c>
+      <c r="E23" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2930,24 +2847,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2964,7 +2881,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2981,7 +2898,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -2998,7 +2915,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -3015,7 +2932,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -3032,7 +2949,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -3049,7 +2966,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -3066,7 +2983,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -3083,7 +3000,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3100,7 +3017,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>11</v>
@@ -3137,24 +3054,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3171,7 +3088,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3188,7 +3105,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3205,7 +3122,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -3222,7 +3139,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -3239,7 +3156,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3256,7 +3173,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <f>B2</f>
@@ -3275,7 +3192,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -3299,14 +3216,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -3314,35 +3233,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>123</v>
+      <c r="E1" s="37" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="26">
+        <v>214</v>
+      </c>
+      <c r="B2" s="24">
         <f>0.00000016*3</f>
         <v>4.8000000000000006E-7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="E2" s="13">
         <f>B2/3</f>
@@ -3351,220 +3270,126 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="10">
-        <v>5</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>25</v>
+        <v>215</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="13">
-        <f>RADIANS(B3)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
+        <v>22</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="25">
-        <v>0.05</v>
+        <v>216</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="14">
-        <f>RADIANS(B4)/SQRT(hr2sec)/3</f>
-        <v>4.8481368110953598E-6</v>
+      <c r="E4" s="1">
+        <f>B4/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>102</v>
+        <v>217</v>
       </c>
       <c r="B5" s="10">
-        <v>20</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="13">
-        <f>RADIANS(B5)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+        <v>77</v>
+      </c>
+      <c r="E5" s="1">
+        <f>B5/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="10">
-        <v>20</v>
+        <v>218</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="13">
-        <f>RADIANS(B6)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+        <v>78</v>
+      </c>
+      <c r="E6" s="1">
+        <f>B6/3</f>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="10">
-        <v>1.5</v>
+        <v>219</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.06</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>84</v>
+        <v>221</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="13">
-        <f>RADIANS(B7)/3600/3</f>
-        <v>2.4240684055476799E-6</v>
+        <v>79</v>
+      </c>
+      <c r="E7" s="1">
+        <f>B7/SQRT(hr2sec)/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="13">
-        <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
-        <v>2.4240684055476799E-6</v>
-      </c>
+      <c r="B8"/>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="10">
-        <v>9</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>1.4544410433286079E-5</v>
-      </c>
+      <c r="B9"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="27">
-        <v>3</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" s="12">
-        <f>B10/3</f>
-        <v>1</v>
-      </c>
+      <c r="B10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="20">
-        <v>3</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="14">
-        <f>B11/3</f>
-        <v>1</v>
-      </c>
+      <c r="B11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B12" s="9">
-        <v>10</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="1">
-        <f>B12/3</f>
-        <v>3.3333333333333335</v>
-      </c>
+      <c r="B12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="9">
-        <v>100</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" s="1">
-        <f>B13/3</f>
-        <v>33.333333333333336</v>
-      </c>
+      <c r="B13"/>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="9">
-        <v>10</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="1">
-        <f>B14/3</f>
-        <v>3.3333333333333335</v>
-      </c>
+      <c r="B14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15"/>
+      <c r="E15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3574,16 +3399,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="6" bestFit="1" customWidth="1"/>
@@ -3591,354 +3417,300 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>123</v>
+      <c r="E1" s="22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4">
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E2" s="12">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
-        <v>1333.3333333333333</v>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B3" s="6">
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E3" s="13">
         <f t="shared" si="0"/>
-        <v>1333.3333333333333</v>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B4" s="6">
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
-        <v>1333.3333333333333</v>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B6" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B7" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B8" s="6">
-        <v>5.0000000000000001E-4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="0"/>
-        <v>1.6666666666666666E-4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B9" s="6">
-        <v>5.0000000000000001E-4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
-        <v>1.6666666666666666E-4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B10" s="6">
-        <v>5.0000000000000001E-4</v>
+        <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="0"/>
-        <v>1.6666666666666666E-4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="6">
-        <f>truthStateParams!$B$5</f>
-        <v>20</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="13">
-        <f>RADIANS(B11)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+      <c r="A11" s="75" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="72">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="77">
+        <f>B11/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="6">
-        <f>truthStateParams!$B$5</f>
-        <v>20</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="13">
-        <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+      <c r="A12" s="75" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" s="72">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="76">
+        <f t="shared" ref="E12:E13" si="1">B12/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="6">
-        <f>truthStateParams!$B$5</f>
-        <v>20</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="13">
+      <c r="A13" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="72">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="76">
         <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="6">
-        <f>truthStateParams!$B$6</f>
-        <v>20</v>
+      <c r="A14" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="24">
+        <v>50</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="13">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" s="11">
+        <f>B14/3</f>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="6">
-        <f>truthStateParams!$B$6</f>
-        <v>20</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="13">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="6">
-        <f>truthStateParams!$B$6</f>
-        <v>20</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="13">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="6">
-        <f>truthStateParams!$B$3</f>
-        <v>5</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="13">
-        <f>RADIANS(B17)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="6">
-        <f>truthStateParams!$B$3</f>
-        <v>5</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="13">
-        <f>RADIANS(B18)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="8">
-        <f>truthStateParams!$B$3</f>
-        <v>5</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" s="14">
-        <f>RADIANS(B19)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
-      </c>
+      <c r="A15" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" s="56">
+        <v>1</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="11">
+        <f>B15/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3950,7 +3722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3964,28 +3738,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>123</v>
+      <c r="E1" s="37" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
-        <v>Q_grav</v>
-      </c>
-      <c r="B2" s="26">
+        <v>Q_nongrav</v>
+      </c>
+      <c r="B2" s="24">
         <f>truthStateParams!B2</f>
         <v>4.8000000000000006E-7</v>
       </c>
@@ -4006,269 +3780,123 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
-        <v>sig_gyro_ss</v>
+        <v>sig_rbias_ss</v>
       </c>
       <c r="B3" s="10">
         <f>truthStateParams!B3</f>
-        <v>5</v>
-      </c>
-      <c r="C3" s="26" t="str">
-        <f>truthStateParams!C3</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D3" s="6" t="str">
-        <f>truthStateParams!D3</f>
-        <v>3-sigma steady-state gyro bias</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" t="s">
+        <v>233</v>
       </c>
       <c r="E3" s="13">
-        <f>RADIANS(B3)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
+        <f>B3/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
-        <v>arw</v>
-      </c>
-      <c r="B4" s="25">
+        <v>sig_abias_ss</v>
+      </c>
+      <c r="B4" s="23">
         <f>truthStateParams!B4</f>
-        <v>0.05</v>
-      </c>
-      <c r="C4" s="8" t="str">
-        <f>truthStateParams!C4</f>
-        <v>deg/sqrt(hr)</v>
-      </c>
-      <c r="D4" s="8" t="str">
-        <f>truthStateParams!D4</f>
-        <v>3-sigma angular random walk</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" t="s">
+        <v>232</v>
       </c>
       <c r="E4" s="14">
-        <f>RADIANS(B4)/SQRT(hr2sec)/3</f>
-        <v>4.8481368110953598E-6</v>
+        <f>B4/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
-        <v>sig_st_ss</v>
+        <v>sig_grav_ss</v>
       </c>
       <c r="B5" s="10">
         <f>truthStateParams!B5</f>
-        <v>20</v>
-      </c>
-      <c r="C5" s="16" t="str">
-        <f>truthStateParams!C5</f>
-        <v>arcsec/axis</v>
-      </c>
-      <c r="D5" s="16" t="str">
-        <f>truthStateParams!D5</f>
-        <v>3-sigma steady-state star camera misalignment</v>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="E5" s="13">
-        <f>RADIANS(B5)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+        <f>B5/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
-        <v>sig_c_ss</v>
+        <v>sig_h_ss</v>
       </c>
       <c r="B6" s="10">
         <f>truthStateParams!B6</f>
-        <v>20</v>
-      </c>
-      <c r="C6" s="16" t="str">
-        <f>truthStateParams!C6</f>
-        <v>arcsec/axis</v>
-      </c>
-      <c r="D6" s="16" t="str">
-        <f>truthStateParams!D6</f>
-        <v>3-sigma steady-state terrain camera misalignment</v>
+        <v>50</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E6" s="13">
-        <f>RADIANS(B6)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+        <f>B6/3</f>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
-        <v>sig_meas_stx</v>
+        <v>vrw</v>
       </c>
       <c r="B7" s="10">
         <f>truthStateParams!B7</f>
-        <v>1.5</v>
-      </c>
-      <c r="C7" s="16" t="str">
-        <f>truthStateParams!C7</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D7" s="16" t="str">
-        <f>truthStateParams!D7</f>
-        <v>3-sigma star camera measurement uncertainty</v>
+        <v>0.06</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>229</v>
       </c>
       <c r="E7" s="13">
-        <f>RADIANS(B7)/3600/3</f>
-        <v>2.4240684055476799E-6</v>
+        <f>B7/3</f>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="str">
-        <f>truthStateParams!A8</f>
-        <v>sig_meas_sty</v>
-      </c>
-      <c r="B8" s="10">
-        <f>truthStateParams!B8</f>
-        <v>1.5</v>
-      </c>
-      <c r="C8" s="16" t="str">
-        <f>truthStateParams!C8</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D8" s="16" t="str">
-        <f>truthStateParams!D8</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E8" s="13">
-        <f t="shared" ref="E8:E9" si="0">RADIANS(B8)/3600/3</f>
-        <v>2.4240684055476799E-6</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="str">
-        <f>truthStateParams!A9</f>
-        <v>sig_meas_stz</v>
-      </c>
-      <c r="B9" s="10">
-        <f>truthStateParams!B9</f>
-        <v>9</v>
-      </c>
-      <c r="C9" s="16" t="str">
-        <f>truthStateParams!C9</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D9" s="16" t="str">
-        <f>truthStateParams!D9</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>1.4544410433286079E-5</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="str">
-        <f>truthStateParams!A10</f>
-        <v>sig_cu</v>
-      </c>
-      <c r="B10" s="27">
-        <f>truthStateParams!B10</f>
-        <v>3</v>
-      </c>
-      <c r="C10" s="46" t="str">
-        <f>truthStateParams!C10</f>
-        <v>pixels</v>
-      </c>
-      <c r="D10" s="46" t="str">
-        <f>truthStateParams!D10</f>
-        <v>3-sigma u component of pixel noise</v>
-      </c>
-      <c r="E10" s="12">
-        <f>B10/3</f>
-        <v>1</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="str">
-        <f>truthStateParams!A11</f>
-        <v>sig_cv</v>
-      </c>
-      <c r="B11" s="20">
-        <f>truthStateParams!B11</f>
-        <v>3</v>
-      </c>
-      <c r="C11" s="17" t="str">
-        <f>truthStateParams!C11</f>
-        <v>pixels</v>
-      </c>
-      <c r="D11" s="17" t="str">
-        <f>truthStateParams!D11</f>
-        <v>3-sigma v component of pixel noise</v>
-      </c>
-      <c r="E11" s="14">
-        <f>B11/3</f>
-        <v>1</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="str">
-        <f>truthStateParams!A12</f>
-        <v>sig_idpos</v>
-      </c>
-      <c r="B12" s="20">
-        <f>truthStateParams!B12</f>
-        <v>10</v>
-      </c>
-      <c r="C12" s="17" t="str">
-        <f>truthStateParams!C12</f>
-        <v>m</v>
-      </c>
-      <c r="D12" s="17" t="str">
-        <f>truthStateParams!D12</f>
-        <v>3-sigma change in inertial position measurement uncertainty</v>
-      </c>
-      <c r="E12" s="14">
-        <f>B12/3</f>
-        <v>3.3333333333333335</v>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="str">
-        <f>truthStateParams!A13</f>
-        <v>sig_loss</v>
-      </c>
-      <c r="B13" s="20">
-        <f>truthStateParams!B13</f>
-        <v>100</v>
-      </c>
-      <c r="C13" s="17" t="str">
-        <f>truthStateParams!C13</f>
-        <v>m</v>
-      </c>
-      <c r="D13" s="17" t="str">
-        <f>truthStateParams!D13</f>
-        <v>3-sigma LOSS feature location uncertainty</v>
-      </c>
-      <c r="E13" s="14">
-        <f>B13/3</f>
-        <v>33.333333333333336</v>
-      </c>
+      <c r="B13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="str">
-        <f>truthStateParams!A14</f>
-        <v>sig_mdpos</v>
-      </c>
-      <c r="B14" s="20">
-        <f>truthStateParams!B14</f>
-        <v>10</v>
-      </c>
-      <c r="C14" s="17" t="str">
-        <f>truthStateParams!C14</f>
-        <v>m</v>
-      </c>
-      <c r="D14" s="17" t="str">
-        <f>truthStateParams!D14</f>
-        <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
-      </c>
-      <c r="E14" s="14">
-        <f>B14/3</f>
-        <v>3.3333333333333335</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4281,13 +3909,14 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D11" sqref="D11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="6" bestFit="1" customWidth="1"/>
@@ -4295,30 +3924,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>123</v>
+      <c r="E1" s="22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="str">
-        <f>truthStateInitialUncertainty!A2</f>
-        <v>sig_rsx</v>
+      <c r="A2" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="B2" s="6">
-        <f>truthStateInitialUncertainty!B2</f>
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>truthStateInitialUncertainty!C2</f>
@@ -4328,20 +3955,18 @@
         <f>truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="38">
         <f t="shared" ref="E2:E10" si="0">B2/3</f>
-        <v>1333.3333333333333</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="str">
-        <f>truthStateInitialUncertainty!A3</f>
-        <v>sig_rsy</v>
+      <c r="A3" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="B3" s="6">
-        <f>truthStateInitialUncertainty!B3</f>
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="C3" s="6" t="str">
         <f>truthStateInitialUncertainty!C3</f>
@@ -4351,20 +3976,18 @@
         <f>truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="38">
         <f t="shared" si="0"/>
-        <v>1333.3333333333333</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="str">
-        <f>truthStateInitialUncertainty!A4</f>
-        <v>sig_rsz</v>
-      </c>
-      <c r="B4" s="6">
-        <f>truthStateInitialUncertainty!B4</f>
-        <v>4000</v>
+      <c r="A4" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="24">
+        <v>400</v>
       </c>
       <c r="C4" s="6" t="str">
         <f>truthStateInitialUncertainty!C4</f>
@@ -4374,20 +3997,18 @@
         <f>truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="38">
         <f t="shared" si="0"/>
-        <v>1333.3333333333333</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="str">
-        <f>truthStateInitialUncertainty!A5</f>
-        <v>sig_vsx</v>
-      </c>
-      <c r="B5" s="6">
-        <f>truthStateInitialUncertainty!B5</f>
-        <v>3</v>
+      <c r="A5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="24">
+        <v>2</v>
       </c>
       <c r="C5" s="6" t="str">
         <f>truthStateInitialUncertainty!C5</f>
@@ -4397,20 +4018,18 @@
         <f>truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="str">
-        <f>truthStateInitialUncertainty!A6</f>
-        <v>sig_vsy</v>
+      <c r="A6" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="B6" s="6">
-        <f>truthStateInitialUncertainty!B6</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="6" t="str">
         <f>truthStateInitialUncertainty!C6</f>
@@ -4420,19 +4039,17 @@
         <f>truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="str">
-        <f>truthStateInitialUncertainty!A7</f>
-        <v>sig_vsz</v>
+      <c r="A7" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="B7" s="6">
-        <f>truthStateInitialUncertainty!B7</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="6" t="str">
         <f>truthStateInitialUncertainty!C7</f>
@@ -4442,274 +4059,166 @@
         <f>truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="38">
         <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="str">
-        <f>truthStateInitialUncertainty!A8</f>
-        <v>sig_ax</v>
-      </c>
-      <c r="B8" s="6">
-        <f>truthStateInitialUncertainty!B8</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="C8" s="6" t="str">
-        <f>truthStateInitialUncertainty!C8</f>
-        <v>rad</v>
-      </c>
-      <c r="D8" s="6" t="str">
-        <f>truthStateInitialUncertainty!D8</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
-      </c>
-      <c r="E8" s="41">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666666E-4</v>
+      <c r="C8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E8" s="38">
+        <f>B8/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="str">
-        <f>truthStateInitialUncertainty!A9</f>
-        <v>sig_ay</v>
-      </c>
-      <c r="B9" s="6">
-        <f>truthStateInitialUncertainty!B9</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="C9" s="6" t="str">
-        <f>truthStateInitialUncertainty!C9</f>
-        <v>rad</v>
-      </c>
-      <c r="D9" s="6" t="str">
-        <f>truthStateInitialUncertainty!D9</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
-      </c>
-      <c r="E9" s="41">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666666E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="str">
-        <f>truthStateInitialUncertainty!A10</f>
-        <v>sig_az</v>
-      </c>
-      <c r="B10" s="6">
-        <f>truthStateInitialUncertainty!B10</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="C10" s="6" t="str">
-        <f>truthStateInitialUncertainty!C10</f>
-        <v>rad</v>
-      </c>
-      <c r="D10" s="6" t="str">
-        <f>truthStateInitialUncertainty!D10</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
-      </c>
-      <c r="E10" s="41">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666666E-4</v>
+      <c r="A9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" s="38">
+        <f t="shared" ref="E9:E10" si="1">B9/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>240</v>
+      </c>
+      <c r="E10" s="38">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="str">
-        <f>truthStateInitialUncertainty!A11</f>
-        <v>sig_thstx</v>
+      <c r="A11" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="B11" s="6">
-        <f>truthStateInitialUncertainty!B11</f>
-        <v>20</v>
-      </c>
-      <c r="C11" s="6" t="str">
-        <f>truthStateInitialUncertainty!C11</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D11" s="6" t="str">
-        <f>truthStateInitialUncertainty!D11</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E11" s="41">
-        <f>RADIANS(B11)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="6">
+        <f>B11/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="str">
-        <f>truthStateInitialUncertainty!A12</f>
-        <v>sig_thsty</v>
+      <c r="A12" s="18" t="s">
+        <v>224</v>
       </c>
       <c r="B12" s="6">
-        <f>truthStateInitialUncertainty!B12</f>
-        <v>20</v>
-      </c>
-      <c r="C12" s="6" t="str">
-        <f>truthStateInitialUncertainty!C12</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D12" s="6" t="str">
-        <f>truthStateInitialUncertainty!D12</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E12" s="41">
-        <f t="shared" ref="E12:E16" si="1">RADIANS(B12)/3600/3</f>
-        <v>3.2320912073969067E-5</v>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:E15" si="2">B12/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="str">
-        <f>truthStateInitialUncertainty!A13</f>
-        <v>sig_thstz</v>
+      <c r="A13" s="18" t="s">
+        <v>225</v>
       </c>
       <c r="B13" s="6">
-        <f>truthStateInitialUncertainty!B13</f>
-        <v>20</v>
-      </c>
-      <c r="C13" s="6" t="str">
-        <f>truthStateInitialUncertainty!C13</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D13" s="6" t="str">
-        <f>truthStateInitialUncertainty!D13</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E13" s="41">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="2"/>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="str">
-        <f>truthStateInitialUncertainty!A14</f>
-        <v>sig_thcx</v>
-      </c>
-      <c r="B14" s="6">
-        <f>truthStateInitialUncertainty!B14</f>
-        <v>20</v>
-      </c>
-      <c r="C14" s="6" t="str">
-        <f>truthStateInitialUncertainty!C14</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D14" s="6" t="str">
-        <f>truthStateInitialUncertainty!D14</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E14" s="41">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
+      <c r="A14" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="16">
+        <v>50</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="str">
-        <f>truthStateInitialUncertainty!A15</f>
-        <v>sig_thcy</v>
-      </c>
-      <c r="B15" s="6">
-        <f>truthStateInitialUncertainty!B15</f>
-        <v>20</v>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>truthStateInitialUncertainty!C15</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D15" s="6" t="str">
-        <f>truthStateInitialUncertainty!D15</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E15" s="41">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
+      <c r="A15" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="str">
-        <f>truthStateInitialUncertainty!A16</f>
-        <v>sig_thcz</v>
-      </c>
-      <c r="B16" s="6">
-        <f>truthStateInitialUncertainty!B16</f>
-        <v>20</v>
-      </c>
-      <c r="C16" s="6" t="str">
-        <f>truthStateInitialUncertainty!C16</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D16" s="6" t="str">
-        <f>truthStateInitialUncertainty!D16</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E16" s="41">
-        <f t="shared" si="1"/>
-        <v>3.2320912073969067E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="str">
-        <f>truthStateInitialUncertainty!A17</f>
-        <v>sig_gyrox</v>
-      </c>
-      <c r="B17" s="6">
-        <f>truthStateInitialUncertainty!B17</f>
-        <v>5</v>
-      </c>
-      <c r="C17" s="6" t="str">
-        <f>truthStateInitialUncertainty!C17</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D17" s="6" t="str">
-        <f>truthStateInitialUncertainty!D17</f>
-        <v>3-sigma initial gyro bias uncertainty</v>
-      </c>
-      <c r="E17" s="41">
-        <f>RADIANS(B17)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
-        <f>truthStateInitialUncertainty!A18</f>
-        <v>sig_gyroy</v>
-      </c>
-      <c r="B18" s="6">
-        <f>truthStateInitialUncertainty!B18</f>
-        <v>5</v>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>truthStateInitialUncertainty!C18</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D18" s="6" t="str">
-        <f>truthStateInitialUncertainty!D18</f>
-        <v>3-sigma initial gyro bias uncertainty</v>
-      </c>
-      <c r="E18" s="41">
-        <f>RADIANS(B18)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="str">
-        <f>truthStateInitialUncertainty!A19</f>
-        <v>sig_gyroz</v>
-      </c>
-      <c r="B19" s="8">
-        <f>truthStateInitialUncertainty!B19</f>
-        <v>5</v>
-      </c>
-      <c r="C19" s="8" t="str">
-        <f>truthStateInitialUncertainty!C19</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D19" s="8" t="str">
-        <f>truthStateInitialUncertainty!D19</f>
-        <v>3-sigma initial gyro bias uncertainty</v>
-      </c>
-      <c r="E19" s="42">
-        <f>RADIANS(B19)/hr2sec/3</f>
-        <v>8.0802280184922667E-6</v>
-      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4722,7 +4231,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4736,25 +4245,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>123</v>
+      <c r="E1" s="37" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B2" s="6">
         <v>100</v>
@@ -4764,9 +4273,9 @@
         <v>m</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="70">
+        <v>102</v>
+      </c>
+      <c r="E2" s="62">
         <f t="shared" ref="E2:E7" si="0">B2</f>
         <v>100</v>
       </c>
@@ -4774,7 +4283,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B3" s="6">
         <v>200</v>
@@ -4784,9 +4293,9 @@
         <v>m</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="70">
+        <v>102</v>
+      </c>
+      <c r="E3" s="62">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
@@ -4794,7 +4303,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B4" s="6">
         <v>300</v>
@@ -4804,9 +4313,9 @@
         <v>m</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="70">
+        <v>102</v>
+      </c>
+      <c r="E4" s="62">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
@@ -4814,7 +4323,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -4824,9 +4333,9 @@
         <v>m/sec</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="70">
+        <v>103</v>
+      </c>
+      <c r="E5" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4834,7 +4343,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -4844,9 +4353,9 @@
         <v>m/sec</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="70">
+        <v>103</v>
+      </c>
+      <c r="E6" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -4854,7 +4363,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
@@ -4864,9 +4373,9 @@
         <v>m/sec</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="70">
+        <v>103</v>
+      </c>
+      <c r="E7" s="62">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -4880,8 +4389,8 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
-        <v>239</v>
+      <c r="A8" s="74" t="s">
+        <v>197</v>
       </c>
       <c r="B8" s="6">
         <v>10</v>
@@ -4890,9 +4399,9 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="70">
+        <v>140</v>
+      </c>
+      <c r="E8" s="62">
         <f>B8</f>
         <v>10</v>
       </c>
@@ -4907,18 +4416,18 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B9" s="26">
+        <v>198</v>
+      </c>
+      <c r="B9" s="24">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E9" s="70">
+        <v>141</v>
+      </c>
+      <c r="E9" s="62">
         <f t="shared" ref="E9:E15" si="1">B9</f>
         <v>6.0000000000000002E-5</v>
       </c>
@@ -4933,18 +4442,18 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B10" s="26">
+        <v>199</v>
+      </c>
+      <c r="B10" s="24">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E10" s="70">
+        <v>141</v>
+      </c>
+      <c r="E10" s="62">
         <f t="shared" si="1"/>
         <v>2.0000000000000002E-5</v>
       </c>
@@ -4959,18 +4468,18 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11" s="26">
+        <v>200</v>
+      </c>
+      <c r="B11" s="24">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E11" s="70">
+        <v>141</v>
+      </c>
+      <c r="E11" s="62">
         <f t="shared" si="1"/>
         <v>3.0000000000000001E-5</v>
       </c>
@@ -4984,8 +4493,8 @@
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="82" t="s">
-        <v>243</v>
+      <c r="A12" s="74" t="s">
+        <v>201</v>
       </c>
       <c r="B12" s="16">
         <v>50</v>
@@ -4994,9 +4503,9 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E12" s="70">
+        <v>142</v>
+      </c>
+      <c r="E12" s="62">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
@@ -5011,18 +4520,18 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>244</v>
+        <v>202</v>
       </c>
       <c r="B13" s="16">
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" s="70">
+        <v>143</v>
+      </c>
+      <c r="E13" s="62">
         <f t="shared" si="1"/>
         <v>3.2699999999999999E-3</v>
       </c>
@@ -5037,18 +4546,18 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>245</v>
+        <v>203</v>
       </c>
       <c r="B14" s="16">
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="E14" s="70">
+        <v>143</v>
+      </c>
+      <c r="E14" s="62">
         <f t="shared" si="1"/>
         <v>3.2699999999999999E-3</v>
       </c>
@@ -5063,18 +4572,18 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>246</v>
+        <v>204</v>
       </c>
       <c r="B15" s="17">
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="71">
+        <v>143</v>
+      </c>
+      <c r="E15" s="63">
         <f t="shared" si="1"/>
         <v>3.2699999999999999E-3</v>
       </c>
@@ -5092,7 +4601,7 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="26"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -5107,7 +4616,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="26"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -5122,7 +4631,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="26"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -5137,7 +4646,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>

</xml_diff>

<commit_message>
Adding+Correcting files for covariance propagation
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7271014-5A80-8846-A5EE-19D443EE36A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818E9E0D-5DF2-E44F-BCF3-B328622D3C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18960" tabRatio="894" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="241">
   <si>
     <t>Value</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>m</t>
-  </si>
-  <si>
-    <t>rad</t>
   </si>
   <si>
     <t>3-sigma angular random walk</t>
@@ -1412,7 +1409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD26"/>
     </sheetView>
   </sheetViews>
@@ -1440,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1463,7 +1460,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="53">
         <v>0.25</v>
@@ -1472,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="54">
         <f t="shared" si="0"/>
@@ -1481,7 +1478,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="53">
         <v>550</v>
@@ -1490,7 +1487,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="54">
         <f t="shared" si="0"/>
@@ -1499,7 +1496,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="53">
         <f>2*PI()/SQRT(B9)*((B11+B12+2*B13)/2)^(3/2)</f>
@@ -1509,7 +1506,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="54">
         <f>B5</f>
@@ -1518,7 +1515,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="55">
         <v>3</v>
@@ -1527,7 +1524,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="54">
         <f>B6</f>
@@ -1536,7 +1533,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="55">
         <v>15</v>
@@ -1545,7 +1542,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="54">
         <f>B7</f>
@@ -1554,7 +1551,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="55">
         <f>12*6</f>
@@ -1564,7 +1561,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="54">
         <f t="shared" si="0"/>
@@ -1573,16 +1570,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="56">
         <v>4902.8010759999997</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="54">
         <f>B9*1000^3</f>
@@ -1591,7 +1588,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="53">
         <v>0</v>
@@ -1600,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="54">
         <f t="shared" si="0"/>
@@ -1609,16 +1606,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="53">
         <v>100</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="54">
         <f>B11*1000</f>
@@ -1627,16 +1624,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="53">
         <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="54">
         <f>B12*1000</f>
@@ -1645,16 +1642,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="53">
         <v>1737.4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="54">
         <f>B13*1000</f>
@@ -1663,16 +1660,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="53">
         <v>1737.4</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="54">
         <f>B14*1000</f>
@@ -1681,16 +1678,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="53">
         <v>13.17635815</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="54">
         <f>RADIANS(B15)/86400</f>
@@ -1699,7 +1696,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="53">
         <v>0</v>
@@ -1708,7 +1705,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="54">
         <f>B16</f>
@@ -1717,7 +1714,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="53">
         <v>0</v>
@@ -1726,7 +1723,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="54">
         <f>B17</f>
@@ -1735,7 +1732,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="53">
         <v>0</v>
@@ -1744,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="54">
         <f>B18</f>
@@ -1753,7 +1750,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19" s="57">
         <v>55</v>
@@ -1762,7 +1759,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E19" s="54">
         <f t="shared" ref="E19:E20" si="1">B19</f>
@@ -1771,7 +1768,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B20" s="57">
         <v>55</v>
@@ -1780,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="54">
         <f t="shared" si="1"/>
@@ -1789,7 +1786,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="55">
         <v>0</v>
@@ -1798,7 +1795,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="54">
         <f t="shared" ref="E21:E23" si="2">B21</f>
@@ -1807,7 +1804,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="55">
         <v>0</v>
@@ -1816,7 +1813,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="54">
         <f t="shared" si="2"/>
@@ -1825,7 +1822,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="55">
         <v>0</v>
@@ -1834,7 +1831,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="54">
         <f t="shared" si="2"/>
@@ -1843,16 +1840,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="53">
         <v>0</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E24" s="54">
         <f t="shared" ref="E24:E26" si="3">RADIANS(B24)</f>
@@ -1861,16 +1858,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" s="53">
         <v>-90</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E25" s="54">
         <f t="shared" si="3"/>
@@ -1879,16 +1876,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B26" s="53">
         <v>30</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="54">
         <f t="shared" si="3"/>
@@ -1897,16 +1894,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="53">
         <v>30</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" s="54">
         <f t="shared" ref="E27:E28" si="4">B27</f>
@@ -1915,7 +1912,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="53">
         <v>0</v>
@@ -1924,7 +1921,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="54">
         <f t="shared" si="4"/>
@@ -1933,16 +1930,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="53">
         <v>19</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E29" s="54">
         <f>B29/1000</f>
@@ -1951,16 +1948,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" s="53">
         <v>7</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" s="54">
         <f>B30*0.000001</f>
@@ -1969,16 +1966,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="53">
         <v>2500</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E31" s="54">
         <f t="shared" ref="E31:E32" si="5">B31</f>
@@ -1987,16 +1984,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="53">
         <v>2500</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E32" s="54">
         <f t="shared" si="5"/>
@@ -2005,7 +2002,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33" s="55">
         <v>5</v>
@@ -2014,7 +2011,7 @@
         <v>4</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" s="54">
         <f>B33</f>
@@ -2023,7 +2020,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B34" s="44">
         <v>0</v>
@@ -2032,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="D34" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="46">
         <f t="shared" ref="E34:E35" si="6">B34</f>
@@ -2041,7 +2038,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="60">
         <v>0</v>
@@ -2050,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E35" s="52">
         <f t="shared" si="6"/>
@@ -2059,7 +2056,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B36" s="55">
         <v>0</v>
@@ -2068,7 +2065,7 @@
         <v>4</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E36" s="54">
         <f t="shared" ref="E36" si="7">B36</f>
@@ -2077,7 +2074,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" s="58">
         <v>0</v>
@@ -2086,7 +2083,7 @@
         <v>4</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E37" s="59">
         <f t="shared" ref="E37:E50" si="8">B37</f>
@@ -2095,16 +2092,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B38" s="2">
         <v>1737.5</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E38" s="1">
         <f>B38*1000</f>
@@ -2113,16 +2110,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" s="2">
         <v>1737.5</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E39" s="1">
         <f>B39*1000</f>
@@ -2131,16 +2128,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40" s="2">
         <v>0</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="8"/>
@@ -2149,16 +2146,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B41" s="2">
         <v>1.62</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="8"/>
@@ -2167,16 +2164,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B42" s="2">
         <v>0</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="8"/>
@@ -2185,16 +2182,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43" s="2">
         <v>0</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="8"/>
@@ -2203,16 +2200,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B44" s="2">
         <v>-1</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="8"/>
@@ -2221,16 +2218,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B45" s="2">
         <v>0</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="8"/>
@@ -2239,16 +2236,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B46" s="2">
         <v>0</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E46" s="1">
         <f>B46*1000</f>
@@ -2257,16 +2254,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B47" s="2">
         <v>1738</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" ref="E47:E48" si="9">B47*1000</f>
@@ -2275,16 +2272,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B48" s="2">
         <v>0</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="9"/>
@@ -2293,16 +2290,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B49" s="72">
         <v>2.7E-6</v>
       </c>
       <c r="C49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="16" t="s">
         <v>169</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>170</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" si="8"/>
@@ -2311,16 +2308,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B50" s="73">
         <v>4904869500000</v>
       </c>
       <c r="C50" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>171</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>172</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="8"/>
@@ -2349,7 +2346,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>60</v>
@@ -2357,7 +2354,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>60</v>
@@ -2365,7 +2362,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <f>hr2min*min2sec</f>
@@ -2374,7 +2371,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>9.81</v>
@@ -2382,7 +2379,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2424,21 +2421,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="28">
         <v>-390</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="66">
         <f>B2*1000</f>
@@ -2447,17 +2444,17 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="30">
         <f>10.3957+1737.5</f>
         <v>1747.8957</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="66">
         <f>B3*1000</f>
@@ -2466,16 +2463,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="32">
+        <v>0</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="32">
-        <v>0</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>72</v>
       </c>
       <c r="E4" s="67">
         <f t="shared" ref="E4" si="0">B4*1000</f>
@@ -2484,16 +2481,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="30">
         <v>1.7</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="66">
         <f>B5*1000</f>
@@ -2502,16 +2499,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="30">
         <v>0</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="66">
         <f>B6*1000</f>
@@ -2520,16 +2517,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="30">
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="66">
         <f>B7*1000</f>
@@ -2538,7 +2535,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" s="40">
         <v>0</v>
@@ -2547,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="68">
         <f>B8</f>
@@ -2556,7 +2553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B9" s="26">
         <v>0</v>
@@ -2565,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E9" s="68">
         <f t="shared" ref="E9:E19" si="1">B9</f>
@@ -2574,7 +2571,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="61">
         <v>0</v>
@@ -2583,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="68">
         <f t="shared" si="1"/>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -2601,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="69">
         <f t="shared" si="1"/>
@@ -2610,7 +2607,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -2619,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" s="70">
         <f>B12</f>
@@ -2628,7 +2625,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" s="61">
         <v>0</v>
@@ -2637,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" s="56">
         <f t="shared" si="1"/>
@@ -2646,7 +2643,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="61">
         <v>0</v>
@@ -2655,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E14" s="56">
         <f t="shared" si="1"/>
@@ -2664,7 +2661,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -2673,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E15" s="25">
         <f t="shared" si="1"/>
@@ -2682,16 +2679,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="64">
         <v>0</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="71">
         <f t="shared" si="1"/>
@@ -2700,7 +2697,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -2709,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="70">
         <f t="shared" si="1"/>
@@ -2718,7 +2715,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -2727,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E18" s="24">
         <f t="shared" si="1"/>
@@ -2736,7 +2733,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B19" s="8">
         <v>0</v>
@@ -2745,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E19" s="25">
         <f t="shared" si="1"/>
@@ -2754,16 +2751,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B20" s="64">
         <v>0</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E20" s="70">
         <f>B20*1000</f>
@@ -2772,7 +2769,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
@@ -2781,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" s="70">
         <f>B21</f>
@@ -2790,7 +2787,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B22" s="16">
         <v>0</v>
@@ -2799,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22" s="70">
         <f t="shared" ref="E22:E23" si="2">B22</f>
@@ -2808,7 +2805,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B23" s="8">
         <v>0</v>
@@ -2817,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E23" s="70">
         <f t="shared" si="2"/>
@@ -2835,7 +2832,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2847,24 +2844,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2881,7 +2878,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2898,7 +2895,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -2915,7 +2912,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -2932,7 +2929,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -2949,7 +2946,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -2966,7 +2963,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -2983,7 +2980,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -3000,7 +2997,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3017,7 +3014,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>11</v>
@@ -3042,7 +3039,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3054,24 +3051,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3088,7 +3085,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3122,7 +3119,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -3139,7 +3136,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -3156,7 +3153,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3173,7 +3170,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <f>B2</f>
@@ -3192,7 +3189,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -3219,7 +3216,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3246,22 +3243,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="24">
         <f>0.00000016*3</f>
         <v>4.8000000000000006E-7</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>106</v>
       </c>
       <c r="E2" s="13">
         <f>B2/3</f>
@@ -3270,7 +3267,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -3279,7 +3276,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1">
         <f>B3/3</f>
@@ -3289,16 +3286,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <f>B4/1000/3</f>
@@ -3307,16 +3304,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" s="10">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1">
         <f>B5/3</f>
@@ -3325,7 +3322,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B6" s="1">
         <v>50</v>
@@ -3334,7 +3331,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="1">
         <f>B6/3</f>
@@ -3343,16 +3340,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" s="1">
         <v>0.06</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="1">
         <f>B7/SQRT(hr2sec)/3</f>
@@ -3399,10 +3396,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3430,12 +3427,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4">
         <v>400</v>
@@ -3444,16 +3441,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="12">
-        <f t="shared" ref="E2:E10" si="0">B2/3</f>
+        <f t="shared" ref="E2:E7" si="0">B2/3</f>
         <v>133.33333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="6">
         <v>400</v>
@@ -3462,7 +3459,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="13">
         <f t="shared" si="0"/>
@@ -3471,7 +3468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="6">
         <v>400</v>
@@ -3480,7 +3477,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
@@ -3489,16 +3486,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
@@ -3507,16 +3504,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="0"/>
@@ -3525,16 +3522,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
@@ -3542,148 +3539,157 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="56">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="13">
-        <f t="shared" si="0"/>
+      <c r="C8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="11">
+        <f>B8/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+      <c r="A9" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="72">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="77">
+        <f>B9/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="13">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+      <c r="A10" s="75" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="72">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="76">
+        <f t="shared" ref="E10:E11" si="1">B10/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="75" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B11" s="72">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
-      </c>
-      <c r="E11" s="77">
-        <f>B11/3</f>
-        <v>2.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
-        <v>224</v>
-      </c>
-      <c r="B12" s="72">
-        <v>6.0000000000000002E-5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D12" t="s">
-        <v>223</v>
-      </c>
-      <c r="E12" s="76">
-        <f t="shared" ref="E12:E13" si="1">B12/3</f>
-        <v>2.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="B13" s="72">
-        <v>6.0000000000000002E-5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>220</v>
-      </c>
-      <c r="D13" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" s="76">
+        <v>222</v>
+      </c>
+      <c r="E11" s="76">
         <f t="shared" si="1"/>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="24">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" s="11">
+        <f>B12/3</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="13">
+        <f>B13/1000/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="B14" s="24">
-        <v>50</v>
+      <c r="A14" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="11">
-        <f>B14/3</f>
-        <v>16.666666666666668</v>
+        <v>173</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="13">
+        <f>B14/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B15" s="56">
+      <c r="A15" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="6">
         <v>1</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="11">
-        <f>B15/3</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="C15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="13">
+        <f>B15/1000/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E22" s="6"/>
@@ -3702,15 +3708,6 @@
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3751,7 +3748,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3788,7 +3785,7 @@
       </c>
       <c r="C3" s="24"/>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3" s="13">
         <f>B3/3</f>
@@ -3807,7 +3804,7 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E4" s="14">
         <f>B4/1000/3</f>
@@ -3826,7 +3823,7 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E5" s="13">
         <f>B5/3</f>
@@ -3845,7 +3842,7 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E6" s="13">
         <f>B6/3</f>
@@ -3863,7 +3860,7 @@
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E7" s="13">
         <f>B7/3</f>
@@ -3906,10 +3903,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3937,12 +3934,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2" s="6">
         <v>400</v>
@@ -3956,14 +3953,14 @@
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
       <c r="E2" s="38">
-        <f t="shared" ref="E2:E10" si="0">B2/3</f>
+        <f t="shared" ref="E2:E7" si="0">B2/3</f>
         <v>133.33333333333334</v>
       </c>
       <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B3" s="6">
         <v>400</v>
@@ -3984,7 +3981,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B4" s="24">
         <v>400</v>
@@ -4005,7 +4002,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5" s="24">
         <v>2</v>
@@ -4026,7 +4023,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -4046,7 +4043,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -4065,160 +4062,151 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>90</v>
+      <c r="A8" s="18" t="s">
+        <v>227</v>
       </c>
       <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>174</v>
+      <c r="C8" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="16">
         <f>B8/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="16">
-        <v>1</v>
+      <c r="A9" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>240</v>
-      </c>
-      <c r="E9" s="38">
-        <f t="shared" ref="E9:E10" si="1">B9/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="16">
-        <v>1</v>
+        <v>222</v>
+      </c>
+      <c r="E9" s="6">
+        <f>B9/3</f>
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="6">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D10" s="79" t="s">
-        <v>240</v>
-      </c>
-      <c r="E10" s="38">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>219</v>
+      </c>
+      <c r="D10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" ref="E10:E12" si="1">B10/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B11" s="6">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E11" s="6">
-        <f>B11/3</f>
+        <f t="shared" si="1"/>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="B12" s="6">
-        <v>6.0000000000000002E-5</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>220</v>
+        <v>226</v>
+      </c>
+      <c r="B12" s="16">
+        <v>50</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
-      </c>
-      <c r="E12" s="6">
-        <f t="shared" ref="E12:E15" si="2">B12/3</f>
-        <v>2.0000000000000002E-5</v>
+        <v>225</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="1"/>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="B13" s="6">
-        <v>6.0000000000000002E-5</v>
+      <c r="A13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" s="6">
-        <f t="shared" si="2"/>
-        <v>2.0000000000000002E-5</v>
+        <v>239</v>
+      </c>
+      <c r="E13" s="38">
+        <f>B13/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>227</v>
+      <c r="A14" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="B14" s="16">
-        <v>50</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="16">
-        <f t="shared" si="2"/>
-        <v>16.666666666666668</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>228</v>
+        <v>239</v>
+      </c>
+      <c r="E14" s="38">
+        <f>B14/1000/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="B15" s="16">
         <v>1</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>241</v>
-      </c>
-      <c r="E15" s="16">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+      <c r="C15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="38">
+        <f>B15/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4258,12 +4246,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6">
         <v>100</v>
@@ -4273,7 +4261,7 @@
         <v>m</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="62">
         <f t="shared" ref="E2:E7" si="0">B2</f>
@@ -4283,7 +4271,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6">
         <v>200</v>
@@ -4293,7 +4281,7 @@
         <v>m</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="62">
         <f t="shared" si="0"/>
@@ -4303,7 +4291,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="6">
         <v>300</v>
@@ -4313,7 +4301,7 @@
         <v>m</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="62">
         <f t="shared" si="0"/>
@@ -4323,7 +4311,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -4333,7 +4321,7 @@
         <v>m/sec</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="62">
         <f t="shared" si="0"/>
@@ -4343,7 +4331,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -4353,7 +4341,7 @@
         <v>m/sec</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="62">
         <f t="shared" si="0"/>
@@ -4363,7 +4351,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
@@ -4373,7 +4361,7 @@
         <v>m/sec</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="62">
         <f t="shared" si="0"/>
@@ -4390,7 +4378,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" s="6">
         <v>10</v>
@@ -4399,7 +4387,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="62">
         <f>B8</f>
@@ -4416,16 +4404,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="24">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="62">
         <f t="shared" ref="E9:E15" si="1">B9</f>
@@ -4442,16 +4430,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10" s="24">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E10" s="62">
         <f t="shared" si="1"/>
@@ -4468,16 +4456,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="24">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E11" s="62">
         <f t="shared" si="1"/>
@@ -4494,7 +4482,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" s="16">
         <v>50</v>
@@ -4503,7 +4491,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" s="62">
         <f t="shared" si="1"/>
@@ -4520,16 +4508,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13" s="16">
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E13" s="62">
         <f t="shared" si="1"/>
@@ -4546,16 +4534,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" s="16">
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="62">
         <f t="shared" si="1"/>
@@ -4572,16 +4560,16 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="17">
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="63">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Finishing up covariance propagation
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evpitts/Fall 2020/Optimal Estimation/Pitts_OptEst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818E9E0D-5DF2-E44F-BCF3-B328622D3C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BBDA69-493A-E94C-9150-7188B416E6D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18960" tabRatio="894" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18940" tabRatio="894" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -3719,8 +3719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3863,8 +3863,8 @@
         <v>228</v>
       </c>
       <c r="E7" s="13">
-        <f>B7/3</f>
-        <v>0.02</v>
+        <f>B7/SQRT(hr2sec)/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3905,7 +3905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>

</xml_diff>